<commit_message>
add code for importing plan data
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="711" firstSheet="4" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="711" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="155">
   <si>
     <t>Notes</t>
   </si>
@@ -1135,12 +1135,6 @@
 Service retirement benefit for tier 3 
 No term assumed after being eligible for retirement
 Refund of member contribution if not eligible to term benefit </t>
-  </si>
-  <si>
-    <t>qxt.fire</t>
-  </si>
-  <si>
-    <t>qxt.plc</t>
   </si>
   <si>
     <t>A5</t>
@@ -1494,6 +1488,21 @@
       <t xml:space="preserve">
 (Do not model for now)</t>
     </r>
+  </si>
+  <si>
+    <t>Healthy mortality table is used for disabled?</t>
+  </si>
+  <si>
+    <t>qxt.fire.yos</t>
+  </si>
+  <si>
+    <t>qxt.plc.yos</t>
+  </si>
+  <si>
+    <t>qxt.fire.age</t>
+  </si>
+  <si>
+    <t>qxt.plc.age</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1698,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1911,6 +1920,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2001,16 +2013,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>513738</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>75555</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323238</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>132705</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2027,7 +2039,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8305800" y="819150"/>
+          <a:off x="3848100" y="685800"/>
           <a:ext cx="4895238" cy="5161905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2331,16 +2343,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>513464</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>113936</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1523114</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>75836</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2357,7 +2369,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8077200" y="533400"/>
+          <a:off x="0" y="1828800"/>
           <a:ext cx="7085714" cy="2914286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2369,16 +2381,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>285109</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171069</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>170809</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>18669</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2395,7 +2407,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7981950" y="3505200"/>
+          <a:off x="609600" y="5448300"/>
           <a:ext cx="5123809" cy="3047619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2672,16 +2684,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>494390</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>151943</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>437240</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>75743</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2698,7 +2710,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3943350" y="762000"/>
+          <a:off x="228600" y="4686300"/>
           <a:ext cx="7276190" cy="3657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2985,16 +2997,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>513738</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>75555</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3011,7 +3023,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8191500" y="438150"/>
+          <a:off x="2819400" y="571500"/>
           <a:ext cx="4895238" cy="5161905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3511,7 +3523,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="A32:XFD32"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,7 +5400,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5436,49 +5448,49 @@
     </row>
     <row r="4" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="D4" s="78" t="s">
         <v>123</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="92" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="95"/>
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="90" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="78" t="s">
-        <v>150</v>
-      </c>
       <c r="E5" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="93" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="92" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="92"/>
+      <c r="G5" s="93"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5545,7 +5557,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5565,7 +5577,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5573,7 +5585,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5581,10 +5593,10 @@
         <v>85</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5785,7 +5797,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5805,7 +5817,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5813,7 +5825,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5821,10 +5833,10 @@
         <v>97</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6088,33 +6100,33 @@
     </row>
     <row r="4" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+        <v>129</v>
+      </c>
+      <c r="B4" s="99" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="5" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="93" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>76</v>
@@ -6122,10 +6134,10 @@
       <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
@@ -6169,7 +6181,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C17"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6192,7 +6204,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6200,7 +6212,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -6210,10 +6222,10 @@
         <v>97</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" s="85" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D5" s="28"/>
     </row>
@@ -6336,7 +6348,7 @@
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6377,7 +6389,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -6410,8 +6422,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6435,7 +6447,9 @@
     </row>
     <row r="5" spans="1:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="8"/>
+      <c r="B5" s="91" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -6469,10 +6483,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6490,7 +6504,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -6546,7 +6560,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="18"/>
     </row>
@@ -6615,7 +6629,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6645,8 +6659,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7005,15 +7019,15 @@
       <c r="A5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="91" t="s">
+      <c r="C5" s="95"/>
+      <c r="D5" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
       <c r="G5" s="43" t="s">
         <v>79</v>
       </c>
@@ -7036,10 +7050,10 @@
       <c r="E6" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="95"/>
+      <c r="G6" s="96"/>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
     </row>
@@ -7063,10 +7077,10 @@
       <c r="C9" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="92"/>
+      <c r="E9" s="93"/>
       <c r="F9" s="39" t="s">
         <v>64</v>
       </c>
@@ -7083,18 +7097,18 @@
       <c r="A11" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="94"/>
-      <c r="D11" s="92" t="s">
+      <c r="C11" s="95"/>
+      <c r="D11" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="92"/>
+      <c r="G11" s="93"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
@@ -7232,7 +7246,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7262,22 +7276,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97" t="s">
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
+      <c r="A6" s="97"/>
       <c r="B6" s="59" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
first working all-tier model for LAFPP
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -2054,6 +2054,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2084,8 +2086,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3692,22 +3692,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99" t="s">
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="98"/>
+      <c r="A6" s="100"/>
       <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
@@ -6429,10 +6429,10 @@
       <c r="E4" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="95"/>
+      <c r="G4" s="97"/>
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
@@ -6450,21 +6450,21 @@
       <c r="E5" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="93"/>
+      <c r="G5" s="95"/>
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -7076,27 +7076,27 @@
       <c r="A4" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="103" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
     </row>
     <row r="5" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="83" t="s">
@@ -7108,10 +7108,10 @@
       <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="97"/>
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
@@ -7443,8 +7443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7699,8 +7699,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7780,7 +7780,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8067,7 +8067,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -8130,22 +8130,22 @@
       <c r="A7" s="80" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="102">
+      <c r="B7" s="92">
         <v>40360</v>
       </c>
       <c r="C7" s="80">
         <v>30</v>
       </c>
-      <c r="D7" s="103">
-        <v>0</v>
-      </c>
-      <c r="E7" s="103">
-        <v>0</v>
-      </c>
-      <c r="F7" s="103">
+      <c r="D7" s="93">
+        <v>0</v>
+      </c>
+      <c r="E7" s="93">
+        <v>0</v>
+      </c>
+      <c r="F7" s="93">
         <v>25</v>
       </c>
-      <c r="G7" s="103">
+      <c r="G7" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8153,22 +8153,22 @@
       <c r="A8" s="80" t="s">
         <v>181</v>
       </c>
-      <c r="B8" s="102">
+      <c r="B8" s="92">
         <v>40725</v>
       </c>
       <c r="C8" s="80">
         <v>30</v>
       </c>
-      <c r="D8" s="103">
-        <v>0</v>
-      </c>
-      <c r="E8" s="103">
-        <v>0</v>
-      </c>
-      <c r="F8" s="103">
+      <c r="D8" s="93">
+        <v>0</v>
+      </c>
+      <c r="E8" s="93">
+        <v>0</v>
+      </c>
+      <c r="F8" s="93">
         <v>26</v>
       </c>
-      <c r="G8" s="103">
+      <c r="G8" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8176,22 +8176,22 @@
       <c r="A9" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="102">
+      <c r="B9" s="92">
         <v>40725</v>
       </c>
       <c r="C9" s="80">
         <v>15</v>
       </c>
-      <c r="D9" s="103">
-        <v>0</v>
-      </c>
-      <c r="E9" s="103">
-        <v>0</v>
-      </c>
-      <c r="F9" s="103">
+      <c r="D9" s="93">
+        <v>0</v>
+      </c>
+      <c r="E9" s="93">
+        <v>0</v>
+      </c>
+      <c r="F9" s="93">
         <v>11</v>
       </c>
-      <c r="G9" s="103">
+      <c r="G9" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8199,22 +8199,22 @@
       <c r="A10" s="80" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="102">
+      <c r="B10" s="92">
         <v>40725</v>
       </c>
       <c r="C10" s="80">
         <v>15</v>
       </c>
-      <c r="D10" s="103">
-        <v>0</v>
-      </c>
-      <c r="E10" s="103">
-        <v>0</v>
-      </c>
-      <c r="F10" s="103">
+      <c r="D10" s="93">
+        <v>0</v>
+      </c>
+      <c r="E10" s="93">
+        <v>0</v>
+      </c>
+      <c r="F10" s="93">
         <v>11</v>
       </c>
-      <c r="G10" s="103">
+      <c r="G10" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8222,22 +8222,22 @@
       <c r="A11" s="80" t="s">
         <v>181</v>
       </c>
-      <c r="B11" s="102">
+      <c r="B11" s="92">
         <v>41091</v>
       </c>
       <c r="C11" s="80">
         <v>30</v>
       </c>
-      <c r="D11" s="103">
-        <v>0</v>
-      </c>
-      <c r="E11" s="103">
-        <v>0</v>
-      </c>
-      <c r="F11" s="103">
+      <c r="D11" s="93">
+        <v>0</v>
+      </c>
+      <c r="E11" s="93">
+        <v>0</v>
+      </c>
+      <c r="F11" s="93">
         <v>27</v>
       </c>
-      <c r="G11" s="103">
+      <c r="G11" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8245,22 +8245,22 @@
       <c r="A12" s="80" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="102">
+      <c r="B12" s="92">
         <v>41456</v>
       </c>
       <c r="C12" s="80">
         <v>30</v>
       </c>
-      <c r="D12" s="103">
-        <v>0</v>
-      </c>
-      <c r="E12" s="103">
-        <v>0</v>
-      </c>
-      <c r="F12" s="103">
+      <c r="D12" s="93">
+        <v>0</v>
+      </c>
+      <c r="E12" s="93">
+        <v>0</v>
+      </c>
+      <c r="F12" s="93">
         <v>28</v>
       </c>
-      <c r="G12" s="103">
+      <c r="G12" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8268,22 +8268,22 @@
       <c r="A13" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="B13" s="102">
+      <c r="B13" s="92">
         <v>41821</v>
       </c>
       <c r="C13" s="80">
         <v>30</v>
       </c>
-      <c r="D13" s="103">
-        <v>0</v>
-      </c>
-      <c r="E13" s="103">
-        <v>0</v>
-      </c>
-      <c r="F13" s="103">
+      <c r="D13" s="93">
+        <v>0</v>
+      </c>
+      <c r="E13" s="93">
+        <v>0</v>
+      </c>
+      <c r="F13" s="93">
         <v>29</v>
       </c>
-      <c r="G13" s="103">
+      <c r="G13" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8291,22 +8291,22 @@
       <c r="A14" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="B14" s="102">
+      <c r="B14" s="92">
         <v>42186</v>
       </c>
       <c r="C14" s="80">
         <v>20</v>
       </c>
-      <c r="D14" s="103">
-        <v>0</v>
-      </c>
-      <c r="E14" s="103">
-        <v>0</v>
-      </c>
-      <c r="F14" s="103">
+      <c r="D14" s="93">
+        <v>0</v>
+      </c>
+      <c r="E14" s="93">
+        <v>0</v>
+      </c>
+      <c r="F14" s="93">
         <v>20</v>
       </c>
-      <c r="G14" s="103">
+      <c r="G14" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8314,22 +8314,22 @@
       <c r="A15" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="102">
+      <c r="B15" s="92">
         <v>42186</v>
       </c>
       <c r="C15" s="80">
         <v>20</v>
       </c>
-      <c r="D15" s="103">
-        <v>0</v>
-      </c>
-      <c r="E15" s="103">
-        <v>0</v>
-      </c>
-      <c r="F15" s="103">
+      <c r="D15" s="93">
+        <v>0</v>
+      </c>
+      <c r="E15" s="93">
+        <v>0</v>
+      </c>
+      <c r="F15" s="93">
         <v>20</v>
       </c>
-      <c r="G15" s="103">
+      <c r="G15" s="93">
         <v>0</v>
       </c>
     </row>
@@ -8373,7 +8373,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8429,15 +8429,15 @@
       <c r="A5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="92" t="s">
+      <c r="C5" s="97"/>
+      <c r="D5" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="42" t="s">
         <v>79</v>
       </c>
@@ -8460,10 +8460,10 @@
       <c r="E6" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="96"/>
+      <c r="G6" s="98"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
     </row>
@@ -8487,10 +8487,10 @@
       <c r="C9" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="93"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="38" t="s">
         <v>64</v>
       </c>
@@ -8502,16 +8502,16 @@
       <c r="A10" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97" t="s">
+      <c r="C10" s="99"/>
+      <c r="D10" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -8522,18 +8522,18 @@
       <c r="A12" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="93" t="s">
+      <c r="C12" s="97"/>
+      <c r="D12" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93" t="s">
+      <c r="E12" s="95"/>
+      <c r="F12" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="93"/>
+      <c r="G12" s="95"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>

</xml_diff>

<commit_message>
checking disability and death benefit
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_LAFPP\Data_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_LAFPP\Data_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Death_sum" sheetId="17" r:id="rId17"/>
     <sheet name="Death_dec" sheetId="5" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3251,23 +3251,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3303,23 +3286,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7339,8 +7305,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7396,7 +7362,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -7443,7 +7409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -7665,7 +7631,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
@@ -7780,7 +7746,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8372,7 +8338,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update contingent annuity for disability benefit
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="2" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="225">
   <si>
     <t>Notes</t>
   </si>
@@ -1160,34 +1160,6 @@
   - yos 20-30: 65% of FAS
   - yos &gt; 30:    75% of FAS
 NonService connected: 40% of FAS</t>
-  </si>
-  <si>
-    <r>
-      <t>Death after retirement
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do not plan to model</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>qxd.fire</t>
@@ -1757,6 +1729,23 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death after retirement
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeling:
+- assuming all disabilities  are service connceted.
+- QSSs' benefits are modeled as a fixed proportion of the pension received by the deceased member immediately preceding the date of death.
+   - Tier 1: 80%  
+   - Tier 2: 80%
+   - Tier 3/4: 60%
+   - Tier 5:  60%
+   - Tier 6: 80% </t>
+  </si>
+  <si>
+    <t>factor.ca.disb</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +1974,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2184,9 +2173,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2271,6 +2257,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2421,13 +2413,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>742164</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>190326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2459,13 +2451,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2475,7 +2467,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8763000" y="7315200"/>
+          <a:off x="8763000" y="9124950"/>
           <a:ext cx="6953250" cy="6115050"/>
           <a:chOff x="6134100" y="1276350"/>
           <a:chExt cx="7219048" cy="6038509"/>
@@ -3916,22 +3908,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
+      <c r="A6" s="109"/>
       <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
@@ -4714,7 +4706,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:G27"/>
+      <selection activeCell="B32" sqref="B32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6639,56 +6631,56 @@
     </row>
     <row r="4" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="D4" s="76" t="s">
         <v>123</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="105" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="107"/>
+      <c r="G4" s="106"/>
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="76" t="s">
+      <c r="F5" s="104" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="105" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="105"/>
+      <c r="G5" s="104"/>
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="112" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
+      <c r="A6" s="111" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -6791,10 +6783,10 @@
         <v>85</v>
       </c>
       <c r="B5" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="79" t="s">
         <v>150</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7031,10 +7023,10 @@
         <v>97</v>
       </c>
       <c r="B5" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="79" t="s">
         <v>152</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7243,10 +7235,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7300,31 +7292,31 @@
       <c r="A4" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="113" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
+      <c r="B4" s="112" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
     </row>
     <row r="5" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="105" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
-        <v>131</v>
+      <c r="A7" s="115" t="s">
+        <v>222</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>76</v>
@@ -7332,10 +7324,10 @@
       <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="107"/>
+      <c r="E7" s="106"/>
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
@@ -7343,26 +7335,39 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+    <row r="8" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="115"/>
+      <c r="B8" s="116" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
@@ -7406,7 +7411,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="85" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -7416,19 +7421,19 @@
       <c r="D3" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="82" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="83" t="s">
-        <v>133</v>
-      </c>
       <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="84">
+      <c r="A6" s="83">
         <v>20</v>
       </c>
       <c r="B6" s="53">
@@ -7441,7 +7446,7 @@
       <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="85">
+      <c r="A7" s="84">
         <v>25</v>
       </c>
       <c r="B7" s="55">
@@ -7454,7 +7459,7 @@
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="85">
+      <c r="A8" s="84">
         <v>30</v>
       </c>
       <c r="B8" s="55">
@@ -7467,7 +7472,7 @@
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="85">
+      <c r="A9" s="84">
         <v>35</v>
       </c>
       <c r="B9" s="55">
@@ -7480,7 +7485,7 @@
       <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="85">
+      <c r="A10" s="84">
         <v>40</v>
       </c>
       <c r="B10" s="55">
@@ -7493,7 +7498,7 @@
       <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="85">
+      <c r="A11" s="84">
         <v>45</v>
       </c>
       <c r="B11" s="55">
@@ -7506,7 +7511,7 @@
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="85">
+      <c r="A12" s="84">
         <v>50</v>
       </c>
       <c r="B12" s="55">
@@ -7519,7 +7524,7 @@
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="85">
+      <c r="A13" s="84">
         <v>55</v>
       </c>
       <c r="B13" s="55">
@@ -7532,7 +7537,7 @@
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="85">
+      <c r="A14" s="84">
         <v>60</v>
       </c>
       <c r="B14" s="55">
@@ -7546,7 +7551,7 @@
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -7563,7 +7568,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -7588,7 +7593,7 @@
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>68</v>
@@ -7597,7 +7602,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>71</v>
@@ -7608,113 +7613,113 @@
     </row>
     <row r="4" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="98" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="101" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="101" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="101" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="98" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="113" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="113"/>
+      <c r="G5" s="101" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="97" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>210</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F4" s="102" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="99" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="102" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" s="102" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" s="114" t="s">
+      <c r="B6" s="98" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="101" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="102" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="98" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="99" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="114" t="s">
-        <v>218</v>
-      </c>
-      <c r="F6" s="114"/>
-      <c r="G6" s="102" t="s">
-        <v>218</v>
-      </c>
-      <c r="H6" s="102" t="s">
-        <v>218</v>
+      <c r="E6" s="113" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="113"/>
+      <c r="G6" s="101" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="101" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
-      <c r="B7" s="99" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="102" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="102" t="s">
-        <v>215</v>
-      </c>
-      <c r="E7" s="114" t="s">
-        <v>219</v>
-      </c>
-      <c r="F7" s="114"/>
-      <c r="G7" s="102" t="s">
-        <v>219</v>
-      </c>
-      <c r="H7" s="102" t="s">
-        <v>221</v>
+      <c r="B7" s="98" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="101" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="101" t="s">
+        <v>214</v>
+      </c>
+      <c r="E7" s="113" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="113"/>
+      <c r="G7" s="101" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="101" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
     </row>
     <row r="9" spans="1:8" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="36"/>
-      <c r="C9" s="92" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="101"/>
+      <c r="C9" s="91" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="100"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -7724,7 +7729,7 @@
     <row r="13" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
-      <c r="G13" s="101"/>
+      <c r="G13" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7747,7 +7752,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7771,8 +7776,8 @@
     </row>
     <row r="5" spans="1:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="88" t="s">
-        <v>149</v>
+      <c r="B5" s="87" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7803,116 +7808,116 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="10" max="12" width="10.5703125" style="93" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="93" customWidth="1"/>
+    <col min="10" max="12" width="10.5703125" style="92" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="92" customWidth="1"/>
     <col min="14" max="14" width="13.140625" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12" style="93" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="93" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" style="93" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" style="93" customWidth="1"/>
+    <col min="17" max="17" width="12" style="92" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="92" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" style="92" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" style="92" customWidth="1"/>
     <col min="21" max="21" width="13.140625" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="J5" s="115" t="s">
-        <v>189</v>
-      </c>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115" t="s">
-        <v>202</v>
-      </c>
-      <c r="R5" s="115"/>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
+      <c r="J5" s="114" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114"/>
+      <c r="Q5" s="114" t="s">
+        <v>201</v>
+      </c>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114"/>
+      <c r="T5" s="114"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="114"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>97</v>
       </c>
       <c r="C6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s">
         <v>195</v>
       </c>
-      <c r="D6" t="s">
-        <v>196</v>
-      </c>
       <c r="E6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G6" t="s">
         <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="J6" s="94" t="s">
+      <c r="K6" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="K6" s="94" t="s">
+      <c r="L6" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="L6" s="94" t="s">
+      <c r="M6" s="93" t="s">
         <v>193</v>
       </c>
-      <c r="M6" s="94" t="s">
-        <v>194</v>
-      </c>
-      <c r="N6" s="94" t="s">
-        <v>198</v>
-      </c>
-      <c r="O6" s="94" t="s">
+      <c r="N6" s="93" t="s">
+        <v>197</v>
+      </c>
+      <c r="O6" s="93" t="s">
+        <v>199</v>
+      </c>
+      <c r="P6" s="93" t="s">
         <v>200</v>
       </c>
-      <c r="P6" s="94" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q6" s="96" t="s">
+      <c r="Q6" s="95" t="s">
+        <v>190</v>
+      </c>
+      <c r="R6" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="R6" s="96" t="s">
+      <c r="S6" s="95" t="s">
         <v>192</v>
       </c>
-      <c r="S6" s="96" t="s">
+      <c r="T6" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="T6" s="96" t="s">
-        <v>194</v>
-      </c>
-      <c r="U6" s="96" t="s">
-        <v>198</v>
-      </c>
-      <c r="V6" s="96" t="s">
+      <c r="U6" s="95" t="s">
+        <v>197</v>
+      </c>
+      <c r="V6" s="95" t="s">
+        <v>199</v>
+      </c>
+      <c r="W6" s="95" t="s">
         <v>200</v>
-      </c>
-      <c r="W6" s="96" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>20</v>
       </c>
-      <c r="C7" s="95">
+      <c r="C7" s="94">
         <v>3.3416560000000002E-4</v>
       </c>
       <c r="D7">
@@ -8854,18 +8859,18 @@
         <f t="shared" si="2"/>
         <v>4.4189770091659719</v>
       </c>
-      <c r="J42" s="93">
+      <c r="J42" s="92">
         <f>E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="K42" s="93">
+      <c r="K42" s="92">
         <f>J42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="L42" s="93">
-        <v>0</v>
-      </c>
-      <c r="M42" s="93">
+      <c r="L42" s="92">
+        <v>0</v>
+      </c>
+      <c r="M42" s="92">
         <f>$E$42</f>
         <v>6.7984261679476479</v>
       </c>
@@ -8919,18 +8924,18 @@
         <f t="shared" si="2"/>
         <v>4.8425189594291114</v>
       </c>
-      <c r="J43" s="93">
+      <c r="J43" s="92">
         <f t="shared" ref="J43:J46" si="4">E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="K43" s="93">
+      <c r="K43" s="92">
         <f>K42*1.05 +J43</f>
         <v>13.936773644292678</v>
       </c>
-      <c r="L43" s="93">
-        <v>0</v>
-      </c>
-      <c r="M43" s="93">
+      <c r="L43" s="92">
+        <v>0</v>
+      </c>
+      <c r="M43" s="92">
         <f t="shared" ref="M43:M106" si="5">$E$42</f>
         <v>6.7984261679476479</v>
       </c>
@@ -8984,18 +8989,18 @@
         <f t="shared" si="2"/>
         <v>5.296327078090318</v>
       </c>
-      <c r="J44" s="93">
+      <c r="J44" s="92">
         <f t="shared" si="4"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="K44" s="93">
+      <c r="K44" s="92">
         <f>K43*1.05 + J44</f>
         <v>21.432038494454961</v>
       </c>
-      <c r="L44" s="93">
-        <v>0</v>
-      </c>
-      <c r="M44" s="93">
+      <c r="L44" s="92">
+        <v>0</v>
+      </c>
+      <c r="M44" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9049,18 +9054,18 @@
         <f t="shared" si="2"/>
         <v>5.7823210346221279</v>
       </c>
-      <c r="J45" s="93">
+      <c r="J45" s="92">
         <f t="shared" si="4"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="K45" s="93">
+      <c r="K45" s="92">
         <f t="shared" ref="K45:K46" si="11">K44*1.05 + J45</f>
         <v>29.30206658712536</v>
       </c>
-      <c r="L45" s="93">
-        <v>0</v>
-      </c>
-      <c r="M45" s="93">
+      <c r="L45" s="92">
+        <v>0</v>
+      </c>
+      <c r="M45" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9114,18 +9119,18 @@
         <f t="shared" si="2"/>
         <v>6.3025345790545186</v>
       </c>
-      <c r="J46" s="93">
+      <c r="J46" s="92">
         <f t="shared" si="4"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="K46" s="93">
+      <c r="K46" s="92">
         <f t="shared" si="11"/>
         <v>37.565596084429274</v>
       </c>
-      <c r="L46" s="93">
-        <v>0</v>
-      </c>
-      <c r="M46" s="93">
+      <c r="L46" s="92">
+        <v>0</v>
+      </c>
+      <c r="M46" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9179,11 +9184,11 @@
         <f t="shared" si="2"/>
         <v>6.9448610739782888</v>
       </c>
-      <c r="L47" s="93">
+      <c r="L47" s="92">
         <f>$E$42 + K46</f>
         <v>44.36402225237692</v>
       </c>
-      <c r="M47" s="93">
+      <c r="M47" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9237,11 +9242,11 @@
         <f t="shared" si="2"/>
         <v>7.5441768629549353</v>
       </c>
-      <c r="L48" s="93">
+      <c r="L48" s="92">
         <f>$E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M48" s="93">
+      <c r="M48" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9295,11 +9300,11 @@
         <f t="shared" si="2"/>
         <v>8.1847583090861988</v>
       </c>
-      <c r="L49" s="93">
+      <c r="L49" s="92">
         <f t="shared" ref="L49:L56" si="12">$E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M49" s="93">
+      <c r="M49" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9353,11 +9358,11 @@
         <f t="shared" si="2"/>
         <v>8.8691734435528868</v>
       </c>
-      <c r="L50" s="93">
+      <c r="L50" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M50" s="93">
+      <c r="M50" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9411,11 +9416,11 @@
         <f t="shared" si="2"/>
         <v>9.2904591821216496</v>
       </c>
-      <c r="L51" s="93">
+      <c r="L51" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M51" s="93">
+      <c r="M51" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9441,7 +9446,7 @@
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="97">
+      <c r="B52" s="96">
         <v>65</v>
       </c>
       <c r="C52">
@@ -9469,11 +9474,11 @@
         <f t="shared" si="2"/>
         <v>9.7317559932724294</v>
       </c>
-      <c r="L52" s="93">
+      <c r="L52" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M52" s="93">
+      <c r="M52" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9489,15 +9494,15 @@
         <f t="shared" si="7"/>
         <v>3.0927925753220662</v>
       </c>
-      <c r="Q52" s="93">
+      <c r="Q52" s="92">
         <f>$E$52</f>
         <v>10.813062214747143</v>
       </c>
-      <c r="R52" s="93">
+      <c r="R52" s="92">
         <f>Q52</f>
         <v>10.813062214747143</v>
       </c>
-      <c r="T52" s="93">
+      <c r="T52" s="92">
         <f t="shared" ref="T52:T106" si="13">$E$52</f>
         <v>10.813062214747143</v>
       </c>
@@ -9543,11 +9548,11 @@
         <f t="shared" si="2"/>
         <v>10.19401440295287</v>
       </c>
-      <c r="L53" s="93">
+      <c r="L53" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M53" s="93">
+      <c r="M53" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9563,15 +9568,15 @@
         <f t="shared" si="7"/>
         <v>2.8459311587651022</v>
       </c>
-      <c r="Q53" s="93">
+      <c r="Q53" s="92">
         <f t="shared" ref="Q53:Q56" si="14">$E$52</f>
         <v>10.813062214747143</v>
       </c>
-      <c r="R53" s="93">
+      <c r="R53" s="92">
         <f>R52*1.05 +Q53</f>
         <v>22.166777540231642</v>
       </c>
-      <c r="T53" s="93">
+      <c r="T53" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9617,11 +9622,11 @@
         <f t="shared" si="2"/>
         <v>10.678230087093132</v>
       </c>
-      <c r="L54" s="93">
+      <c r="L54" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M54" s="93">
+      <c r="M54" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9637,15 +9642,15 @@
         <f t="shared" si="7"/>
         <v>2.61617031790247</v>
       </c>
-      <c r="Q54" s="93">
+      <c r="Q54" s="92">
         <f t="shared" si="14"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="R54" s="93">
+      <c r="R54" s="92">
         <f>R53*1.05 + Q54</f>
         <v>34.088178631990367</v>
       </c>
-      <c r="T54" s="93">
+      <c r="T54" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9691,11 +9696,11 @@
         <f t="shared" si="2"/>
         <v>11.185446016230058</v>
       </c>
-      <c r="L55" s="93">
+      <c r="L55" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M55" s="93">
+      <c r="M55" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9711,15 +9716,15 @@
         <f t="shared" si="7"/>
         <v>2.4024576619956037</v>
       </c>
-      <c r="Q55" s="93">
+      <c r="Q55" s="92">
         <f t="shared" si="14"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="R55" s="93">
+      <c r="R55" s="92">
         <f t="shared" ref="R55:R56" si="16">R54*1.05 + Q55</f>
         <v>46.605649778337025</v>
       </c>
-      <c r="T55" s="93">
+      <c r="T55" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9765,11 +9770,11 @@
         <f t="shared" si="2"/>
         <v>11.716754702000985</v>
       </c>
-      <c r="L56" s="93">
+      <c r="L56" s="92">
         <f t="shared" si="12"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M56" s="93">
+      <c r="M56" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9785,15 +9790,15 @@
         <f t="shared" si="7"/>
         <v>2.2031082478198898</v>
       </c>
-      <c r="Q56" s="93">
+      <c r="Q56" s="92">
         <f t="shared" si="14"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="R56" s="93">
+      <c r="R56" s="92">
         <f t="shared" si="16"/>
         <v>59.748994482001017</v>
       </c>
-      <c r="T56" s="93">
+      <c r="T56" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9839,11 +9844,11 @@
         <f t="shared" si="2"/>
         <v>12.273300550346033</v>
       </c>
-      <c r="L57" s="93">
+      <c r="L57" s="92">
         <f>$E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M57" s="93">
+      <c r="M57" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9859,11 +9864,11 @@
         <f t="shared" si="7"/>
         <v>2.0167671825163049</v>
       </c>
-      <c r="S57" s="93">
+      <c r="S57" s="92">
         <f>R56+$E$52</f>
         <v>70.562056696748158</v>
       </c>
-      <c r="T57" s="93">
+      <c r="T57" s="92">
         <f>$E$52</f>
         <v>10.813062214747143</v>
       </c>
@@ -9891,11 +9896,11 @@
         <f t="shared" si="0"/>
         <v>0.82856323681831068</v>
       </c>
-      <c r="L58" s="93">
+      <c r="L58" s="92">
         <f t="shared" ref="L58:L106" si="17">$E$42</f>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M58" s="93">
+      <c r="M58" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9911,11 +9916,11 @@
         <f t="shared" si="7"/>
         <v>1.8430065541042151</v>
       </c>
-      <c r="S58" s="93">
+      <c r="S58" s="92">
         <f>$E$52</f>
         <v>10.813062214747143</v>
       </c>
-      <c r="T58" s="93">
+      <c r="T58" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9943,11 +9948,11 @@
         <f t="shared" si="0"/>
         <v>0.81235323675594462</v>
       </c>
-      <c r="L59" s="93">
+      <c r="L59" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M59" s="93">
+      <c r="M59" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -9963,11 +9968,11 @@
         <f t="shared" si="7"/>
         <v>1.680883719605589</v>
       </c>
-      <c r="S59" s="93">
+      <c r="S59" s="92">
         <f t="shared" ref="S59:S106" si="18">$E$52</f>
         <v>10.813062214747143</v>
       </c>
-      <c r="T59" s="93">
+      <c r="T59" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -9995,11 +10000,11 @@
         <f t="shared" si="0"/>
         <v>0.79465093201826931</v>
       </c>
-      <c r="L60" s="93">
+      <c r="L60" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M60" s="93">
+      <c r="M60" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10015,11 +10020,11 @@
         <f t="shared" si="7"/>
         <v>1.5295394697233526</v>
       </c>
-      <c r="S60" s="93">
+      <c r="S60" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T60" s="93">
+      <c r="T60" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10047,11 +10052,11 @@
         <f t="shared" si="0"/>
         <v>0.77533244251717404</v>
       </c>
-      <c r="L61" s="93">
+      <c r="L61" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M61" s="93">
+      <c r="M61" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10067,11 +10072,11 @@
         <f t="shared" si="7"/>
         <v>1.3882375386379853</v>
       </c>
-      <c r="S61" s="93">
+      <c r="S61" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T61" s="93">
+      <c r="T61" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10099,11 +10104,11 @@
         <f t="shared" si="0"/>
         <v>0.75429624270826012</v>
       </c>
-      <c r="L62" s="93">
+      <c r="L62" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M62" s="93">
+      <c r="M62" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10119,11 +10124,11 @@
         <f t="shared" si="7"/>
         <v>1.2563461326872842</v>
       </c>
-      <c r="S62" s="93">
+      <c r="S62" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T62" s="93">
+      <c r="T62" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10151,11 +10156,11 @@
         <f t="shared" si="0"/>
         <v>0.73148587333503878</v>
       </c>
-      <c r="L63" s="93">
+      <c r="L63" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M63" s="93">
+      <c r="M63" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10171,11 +10176,11 @@
         <f t="shared" si="7"/>
         <v>1.1333520692702026</v>
       </c>
-      <c r="S63" s="93">
+      <c r="S63" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T63" s="93">
+      <c r="T63" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10203,11 +10208,11 @@
         <f t="shared" si="0"/>
         <v>0.70688041756920683</v>
       </c>
-      <c r="L64" s="93">
+      <c r="L64" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M64" s="93">
+      <c r="M64" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10223,11 +10228,11 @@
         <f t="shared" si="7"/>
         <v>1.0188174740132456</v>
       </c>
-      <c r="S64" s="93">
+      <c r="S64" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T64" s="93">
+      <c r="T64" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10255,11 +10260,11 @@
         <f t="shared" si="0"/>
         <v>0.68045800767369868</v>
       </c>
-      <c r="L65" s="93">
+      <c r="L65" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M65" s="93">
+      <c r="M65" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10275,11 +10280,11 @@
         <f t="shared" si="7"/>
         <v>0.91231181507125081</v>
       </c>
-      <c r="S65" s="93">
+      <c r="S65" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T65" s="93">
+      <c r="T65" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10307,11 +10312,11 @@
         <f t="shared" si="0"/>
         <v>0.65219102597804091</v>
       </c>
-      <c r="L66" s="93">
+      <c r="L66" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M66" s="93">
+      <c r="M66" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10327,11 +10332,11 @@
         <f t="shared" si="7"/>
         <v>0.81340778474747322</v>
       </c>
-      <c r="S66" s="93">
+      <c r="S66" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T66" s="93">
+      <c r="T66" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10359,11 +10364,11 @@
         <f t="shared" si="0"/>
         <v>0.62208579906438133</v>
       </c>
-      <c r="L67" s="93">
+      <c r="L67" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M67" s="93">
+      <c r="M67" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10379,11 +10384,11 @@
         <f t="shared" si="7"/>
         <v>0.72173094903319601</v>
       </c>
-      <c r="S67" s="93">
+      <c r="S67" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T67" s="93">
+      <c r="T67" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10411,11 +10416,11 @@
         <f t="shared" si="0"/>
         <v>0.58994718895047804</v>
       </c>
-      <c r="L68" s="93">
+      <c r="L68" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M68" s="93">
+      <c r="M68" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10431,11 +10436,11 @@
         <f t="shared" si="7"/>
         <v>0.63669246970930993</v>
       </c>
-      <c r="S68" s="93">
+      <c r="S68" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T68" s="93">
+      <c r="T68" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10463,11 +10468,11 @@
         <f t="shared" si="0"/>
         <v>0.55589613558373874</v>
       </c>
-      <c r="L69" s="93">
+      <c r="L69" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M69" s="93">
+      <c r="M69" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10483,11 +10488,11 @@
         <f t="shared" si="7"/>
         <v>0.55808682239463647</v>
       </c>
-      <c r="S69" s="93">
+      <c r="S69" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T69" s="93">
+      <c r="T69" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10515,11 +10520,11 @@
         <f t="shared" si="0"/>
         <v>0.52013014072015107</v>
       </c>
-      <c r="L70" s="93">
+      <c r="L70" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M70" s="93">
+      <c r="M70" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10535,11 +10540,11 @@
         <f t="shared" si="7"/>
         <v>0.48574872573970462</v>
       </c>
-      <c r="S70" s="93">
+      <c r="S70" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T70" s="93">
+      <c r="T70" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10567,11 +10572,11 @@
         <f t="shared" si="0"/>
         <v>0.48291255139771205</v>
       </c>
-      <c r="L71" s="93">
+      <c r="L71" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M71" s="93">
+      <c r="M71" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10587,11 +10592,11 @@
         <f t="shared" si="7"/>
         <v>0.41952676950903162</v>
       </c>
-      <c r="S71" s="93">
+      <c r="S71" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T71" s="93">
+      <c r="T71" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10619,11 +10624,11 @@
         <f t="shared" si="0"/>
         <v>0.44455624777516756</v>
       </c>
-      <c r="L72" s="93">
+      <c r="L72" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M72" s="93">
+      <c r="M72" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10639,11 +10644,11 @@
         <f t="shared" si="7"/>
         <v>0.35926047394183436</v>
       </c>
-      <c r="S72" s="93">
+      <c r="S72" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T72" s="93">
+      <c r="T72" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10671,11 +10676,11 @@
         <f t="shared" ref="D73:D106" si="19">D72*(1-C72)</f>
         <v>0.40540807054563471</v>
       </c>
-      <c r="L73" s="93">
+      <c r="L73" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M73" s="93">
+      <c r="M73" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10691,11 +10696,11 @@
         <f t="shared" si="7"/>
         <v>0.30476609196296539</v>
       </c>
-      <c r="S73" s="93">
+      <c r="S73" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T73" s="93">
+      <c r="T73" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10723,11 +10728,11 @@
         <f t="shared" si="19"/>
         <v>0.36496345429910237</v>
       </c>
-      <c r="L74" s="93">
+      <c r="L74" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M74" s="93">
+      <c r="M74" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10743,11 +10748,11 @@
         <f t="shared" si="7"/>
         <v>0.25522027380745999</v>
       </c>
-      <c r="S74" s="93">
+      <c r="S74" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T74" s="93">
+      <c r="T74" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10775,11 +10780,11 @@
         <f t="shared" si="19"/>
         <v>0.32375153217106822</v>
       </c>
-      <c r="L75" s="93">
+      <c r="L75" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M75" s="93">
+      <c r="M75" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10795,11 +10800,11 @@
         <f t="shared" si="7"/>
         <v>0.21060523391108546</v>
       </c>
-      <c r="S75" s="93">
+      <c r="S75" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T75" s="93">
+      <c r="T75" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10827,11 +10832,11 @@
         <f t="shared" si="19"/>
         <v>0.28244011143023273</v>
       </c>
-      <c r="L76" s="93">
+      <c r="L76" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M76" s="93">
+      <c r="M76" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10847,11 +10852,11 @@
         <f t="shared" si="7"/>
         <v>0.170913055150927</v>
       </c>
-      <c r="S76" s="93">
+      <c r="S76" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T76" s="93">
+      <c r="T76" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10879,11 +10884,11 @@
         <f t="shared" si="19"/>
         <v>0.24182729908718817</v>
       </c>
-      <c r="L77" s="93">
+      <c r="L77" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M77" s="93">
+      <c r="M77" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10899,11 +10904,11 @@
         <f t="shared" si="7"/>
         <v>0.13612745476963467</v>
       </c>
-      <c r="S77" s="93">
+      <c r="S77" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T77" s="93">
+      <c r="T77" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10931,11 +10936,11 @@
         <f t="shared" si="19"/>
         <v>0.20310084780351195</v>
       </c>
-      <c r="L78" s="93">
+      <c r="L78" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M78" s="93">
+      <c r="M78" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -10951,11 +10956,11 @@
         <f t="shared" si="7"/>
         <v>0.10635151259503718</v>
       </c>
-      <c r="S78" s="93">
+      <c r="S78" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T78" s="93">
+      <c r="T78" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -10983,11 +10988,11 @@
         <f t="shared" si="19"/>
         <v>0.16704293264795009</v>
       </c>
-      <c r="L79" s="93">
+      <c r="L79" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M79" s="93">
+      <c r="M79" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11003,11 +11008,11 @@
         <f t="shared" si="7"/>
         <v>8.1367613149169779E-2</v>
       </c>
-      <c r="S79" s="93">
+      <c r="S79" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T79" s="93">
+      <c r="T79" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11035,11 +11040,11 @@
         <f t="shared" si="19"/>
         <v>0.13433350212469566</v>
       </c>
-      <c r="L80" s="93">
+      <c r="L80" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M80" s="93">
+      <c r="M80" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11055,11 +11060,11 @@
         <f t="shared" si="7"/>
         <v>6.0869445207679951E-2</v>
       </c>
-      <c r="S80" s="93">
+      <c r="S80" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T80" s="93">
+      <c r="T80" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11087,11 +11092,11 @@
         <f t="shared" si="19"/>
         <v>0.10547923743049588</v>
       </c>
-      <c r="L81" s="93">
+      <c r="L81" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M81" s="93">
+      <c r="M81" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11107,11 +11112,11 @@
         <f t="shared" si="7"/>
         <v>4.4460416152917001E-2</v>
       </c>
-      <c r="S81" s="93">
+      <c r="S81" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T81" s="93">
+      <c r="T81" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11139,11 +11144,11 @@
         <f t="shared" si="19"/>
         <v>8.0763327010334174E-2</v>
       </c>
-      <c r="L82" s="93">
+      <c r="L82" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M82" s="93">
+      <c r="M82" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11159,11 +11164,11 @@
         <f t="shared" si="7"/>
         <v>3.1667390608636568E-2</v>
       </c>
-      <c r="S82" s="93">
+      <c r="S82" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T82" s="93">
+      <c r="T82" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11191,11 +11196,11 @@
         <f t="shared" si="19"/>
         <v>6.0228312276585545E-2</v>
       </c>
-      <c r="L83" s="93">
+      <c r="L83" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M83" s="93">
+      <c r="M83" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11211,11 +11216,11 @@
         <f t="shared" si="7"/>
         <v>2.1967989233155204E-2</v>
       </c>
-      <c r="S83" s="93">
+      <c r="S83" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T83" s="93">
+      <c r="T83" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11243,11 +11248,11 @@
         <f t="shared" si="19"/>
         <v>4.3692973821657315E-2</v>
       </c>
-      <c r="L84" s="93">
+      <c r="L84" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M84" s="93">
+      <c r="M84" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11263,11 +11268,11 @@
         <f t="shared" si="7"/>
         <v>1.482493349748654E-2</v>
       </c>
-      <c r="S84" s="93">
+      <c r="S84" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T84" s="93">
+      <c r="T84" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11295,11 +11300,11 @@
         <f t="shared" si="19"/>
         <v>3.1079476740244239E-2</v>
       </c>
-      <c r="L85" s="93">
+      <c r="L85" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M85" s="93">
+      <c r="M85" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11315,11 +11320,11 @@
         <f t="shared" si="7"/>
         <v>9.8094889738961286E-3</v>
       </c>
-      <c r="S85" s="93">
+      <c r="S85" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T85" s="93">
+      <c r="T85" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11347,11 +11352,11 @@
         <f t="shared" si="19"/>
         <v>2.1473236209615078E-2</v>
       </c>
-      <c r="L86" s="93">
+      <c r="L86" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M86" s="93">
+      <c r="M86" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11367,11 +11372,11 @@
         <f t="shared" si="7"/>
         <v>6.3046607473727888E-3</v>
       </c>
-      <c r="S86" s="93">
+      <c r="S86" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T86" s="93">
+      <c r="T86" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11399,11 +11404,11 @@
         <f t="shared" si="19"/>
         <v>1.4547741507732977E-2</v>
       </c>
-      <c r="L87" s="93">
+      <c r="L87" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M87" s="93">
+      <c r="M87" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11419,11 +11424,11 @@
         <f t="shared" si="7"/>
         <v>3.9732997707342494E-3</v>
       </c>
-      <c r="S87" s="93">
+      <c r="S87" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T87" s="93">
+      <c r="T87" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11451,11 +11456,11 @@
         <f t="shared" si="19"/>
         <v>9.5553150262579004E-3</v>
       </c>
-      <c r="L88" s="93">
+      <c r="L88" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M88" s="93">
+      <c r="M88" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11471,11 +11476,11 @@
         <f t="shared" si="7"/>
         <v>2.4276848160192815E-3</v>
       </c>
-      <c r="S88" s="93">
+      <c r="S88" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T88" s="93">
+      <c r="T88" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11503,11 +11508,11 @@
         <f t="shared" si="19"/>
         <v>6.1567784145890453E-3</v>
       </c>
-      <c r="L89" s="93">
+      <c r="L89" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M89" s="93">
+      <c r="M89" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11523,11 +11528,11 @@
         <f t="shared" si="7"/>
         <v>1.4550983606719764E-3</v>
       </c>
-      <c r="S89" s="93">
+      <c r="S89" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T89" s="93">
+      <c r="T89" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11555,11 +11560,11 @@
         <f t="shared" si="19"/>
         <v>3.8498272922810836E-3</v>
       </c>
-      <c r="L90" s="93">
+      <c r="L90" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M90" s="93">
+      <c r="M90" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11575,11 +11580,11 @@
         <f t="shared" si="7"/>
         <v>8.4639211880216847E-4</v>
       </c>
-      <c r="S90" s="93">
+      <c r="S90" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T90" s="93">
+      <c r="T90" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11607,11 +11612,11 @@
         <f t="shared" si="19"/>
         <v>2.3735383096026431E-3</v>
       </c>
-      <c r="L91" s="93">
+      <c r="L91" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M91" s="93">
+      <c r="M91" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11627,11 +11632,11 @@
         <f t="shared" si="7"/>
         <v>4.8542053578656802E-4</v>
       </c>
-      <c r="S91" s="93">
+      <c r="S91" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T91" s="93">
+      <c r="T91" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11659,11 +11664,11 @@
         <f t="shared" si="19"/>
         <v>1.429140645748086E-3</v>
       </c>
-      <c r="L92" s="93">
+      <c r="L92" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M92" s="93">
+      <c r="M92" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11679,11 +11684,11 @@
         <f t="shared" si="7"/>
         <v>2.7188697719497088E-4</v>
       </c>
-      <c r="S92" s="93">
+      <c r="S92" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T92" s="93">
+      <c r="T92" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11711,11 +11716,11 @@
         <f t="shared" si="19"/>
         <v>8.5748438744885159E-4</v>
       </c>
-      <c r="L93" s="93">
+      <c r="L93" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M93" s="93">
+      <c r="M93" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11731,11 +11736,11 @@
         <f t="shared" si="7"/>
         <v>1.5175087099254185E-4</v>
       </c>
-      <c r="S93" s="93">
+      <c r="S93" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T93" s="93">
+      <c r="T93" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11763,11 +11768,11 @@
         <f t="shared" si="19"/>
         <v>5.1449063246931091E-4</v>
       </c>
-      <c r="L94" s="93">
+      <c r="L94" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M94" s="93">
+      <c r="M94" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11783,11 +11788,11 @@
         <f t="shared" si="7"/>
         <v>8.4698160553976846E-5</v>
       </c>
-      <c r="S94" s="93">
+      <c r="S94" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T94" s="93">
+      <c r="T94" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11815,11 +11820,11 @@
         <f t="shared" si="19"/>
         <v>3.0869437948158654E-4</v>
       </c>
-      <c r="L95" s="93">
+      <c r="L95" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M95" s="93">
+      <c r="M95" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11835,11 +11840,11 @@
         <f t="shared" si="7"/>
         <v>4.7273391937103357E-5</v>
       </c>
-      <c r="S95" s="93">
+      <c r="S95" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T95" s="93">
+      <c r="T95" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11867,11 +11872,11 @@
         <f t="shared" si="19"/>
         <v>1.8521662768895193E-4</v>
       </c>
-      <c r="L96" s="93">
+      <c r="L96" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M96" s="93">
+      <c r="M96" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11887,11 +11892,11 @@
         <f t="shared" si="7"/>
         <v>2.6385148988150714E-5</v>
       </c>
-      <c r="S96" s="93">
+      <c r="S96" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T96" s="93">
+      <c r="T96" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11919,11 +11924,11 @@
         <f t="shared" si="19"/>
         <v>1.1112997661337116E-4</v>
       </c>
-      <c r="L97" s="93">
+      <c r="L97" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M97" s="93">
+      <c r="M97" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11939,11 +11944,11 @@
         <f t="shared" si="7"/>
         <v>1.4726594784084121E-5</v>
       </c>
-      <c r="S97" s="93">
+      <c r="S97" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T97" s="93">
+      <c r="T97" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -11971,11 +11976,11 @@
         <f t="shared" si="19"/>
         <v>6.6677985968022693E-5</v>
       </c>
-      <c r="L98" s="93">
+      <c r="L98" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M98" s="93">
+      <c r="M98" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -11991,11 +11996,11 @@
         <f t="shared" si="7"/>
         <v>8.2194947632097419E-6</v>
       </c>
-      <c r="S98" s="93">
+      <c r="S98" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T98" s="93">
+      <c r="T98" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12023,11 +12028,11 @@
         <f t="shared" si="19"/>
         <v>4.0006791580813616E-5</v>
       </c>
-      <c r="L99" s="93">
+      <c r="L99" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M99" s="93">
+      <c r="M99" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12043,11 +12048,11 @@
         <f t="shared" si="7"/>
         <v>4.587624984117065E-6</v>
       </c>
-      <c r="S99" s="93">
+      <c r="S99" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T99" s="93">
+      <c r="T99" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12075,11 +12080,11 @@
         <f t="shared" si="19"/>
         <v>2.400407494848817E-5</v>
       </c>
-      <c r="L100" s="93">
+      <c r="L100" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M100" s="93">
+      <c r="M100" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12095,11 +12100,11 @@
         <f t="shared" si="7"/>
         <v>2.5605348748560373E-6</v>
       </c>
-      <c r="S100" s="93">
+      <c r="S100" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T100" s="93">
+      <c r="T100" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12127,11 +12132,11 @@
         <f t="shared" si="19"/>
         <v>1.4402444969092902E-5</v>
       </c>
-      <c r="L101" s="93">
+      <c r="L101" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M101" s="93">
+      <c r="M101" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12147,11 +12152,11 @@
         <f t="shared" si="7"/>
         <v>1.429135744105695E-6</v>
       </c>
-      <c r="S101" s="93">
+      <c r="S101" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T101" s="93">
+      <c r="T101" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12179,11 +12184,11 @@
         <f t="shared" si="19"/>
         <v>8.6414669814557416E-6</v>
       </c>
-      <c r="L102" s="93">
+      <c r="L102" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M102" s="93">
+      <c r="M102" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12199,11 +12204,11 @@
         <f t="shared" si="7"/>
         <v>7.9765715950085294E-7</v>
       </c>
-      <c r="S102" s="93">
+      <c r="S102" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T102" s="93">
+      <c r="T102" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12231,11 +12236,11 @@
         <f t="shared" si="19"/>
         <v>5.1848801888734449E-6</v>
       </c>
-      <c r="L103" s="93">
+      <c r="L103" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M103" s="93">
+      <c r="M103" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12251,11 +12256,11 @@
         <f t="shared" si="7"/>
         <v>4.4520399600047596E-7</v>
       </c>
-      <c r="S103" s="93">
+      <c r="S103" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T103" s="93">
+      <c r="T103" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12283,11 +12288,11 @@
         <f t="shared" si="19"/>
         <v>3.1109281133240667E-6</v>
       </c>
-      <c r="L104" s="93">
+      <c r="L104" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M104" s="93">
+      <c r="M104" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12303,11 +12308,11 @@
         <f t="shared" si="7"/>
         <v>2.4848595125607966E-7</v>
       </c>
-      <c r="S104" s="93">
+      <c r="S104" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T104" s="93">
+      <c r="T104" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12335,11 +12340,11 @@
         <f t="shared" si="19"/>
         <v>1.8665568679944399E-6</v>
       </c>
-      <c r="L105" s="93">
+      <c r="L105" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M105" s="93">
+      <c r="M105" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12355,11 +12360,11 @@
         <f t="shared" si="7"/>
         <v>1.3868983325920723E-7</v>
       </c>
-      <c r="S105" s="93">
+      <c r="S105" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T105" s="93">
+      <c r="T105" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12387,11 +12392,11 @@
         <f t="shared" si="19"/>
         <v>1.1199341207966639E-6</v>
       </c>
-      <c r="L106" s="93">
+      <c r="L106" s="92">
         <f t="shared" si="17"/>
         <v>6.7984261679476479</v>
       </c>
-      <c r="M106" s="93">
+      <c r="M106" s="92">
         <f t="shared" si="5"/>
         <v>6.7984261679476479</v>
       </c>
@@ -12407,11 +12412,11 @@
         <f t="shared" si="7"/>
         <v>7.7408279028394735E-8</v>
       </c>
-      <c r="S106" s="93">
+      <c r="S106" s="92">
         <f t="shared" si="18"/>
         <v>10.813062214747143</v>
       </c>
-      <c r="T106" s="93">
+      <c r="T106" s="92">
         <f t="shared" si="13"/>
         <v>10.813062214747143</v>
       </c>
@@ -12429,8 +12434,8 @@
       </c>
     </row>
     <row r="108" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="N108" s="93" t="s">
-        <v>199</v>
+      <c r="N108" s="92" t="s">
+        <v>198</v>
       </c>
       <c r="O108">
         <f>SUM(O42:O106)</f>
@@ -12440,8 +12445,8 @@
         <f>SUM(P42:P106)</f>
         <v>80.573925783148752</v>
       </c>
-      <c r="U108" s="93" t="s">
-        <v>203</v>
+      <c r="U108" s="92" t="s">
+        <v>202</v>
       </c>
       <c r="V108">
         <f>SUM(V42:V106)</f>
@@ -12474,20 +12479,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>87</v>
       </c>
@@ -12495,193 +12503,214 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="88" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="G6" s="88" t="s">
+        <v>224</v>
+      </c>
+      <c r="H6" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="88" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="89" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="89" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="89" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="89" t="s">
-        <v>171</v>
-      </c>
-      <c r="G6" s="89" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6" s="89" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
+      <c r="B7" s="88">
+        <v>20</v>
+      </c>
+      <c r="C7" s="88">
+        <v>0</v>
+      </c>
+      <c r="D7" s="88">
+        <v>1</v>
+      </c>
+      <c r="E7" s="88">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F7" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="88">
+        <v>0.8</v>
+      </c>
+      <c r="H7" s="88">
+        <v>50</v>
+      </c>
+      <c r="I7" s="88">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="89">
+      <c r="B8" s="88">
         <v>20</v>
       </c>
-      <c r="C7" s="89">
-        <v>0</v>
-      </c>
-      <c r="D7" s="89">
+      <c r="C8" s="88">
+        <v>0</v>
+      </c>
+      <c r="D8" s="88">
         <v>1</v>
       </c>
-      <c r="E7" s="89">
-        <v>3.2500000000000001E-2</v>
-      </c>
-      <c r="F7" s="89">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="89">
+      <c r="E8" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="88">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G8" s="88">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="88">
         <v>50</v>
       </c>
-      <c r="H7" s="89">
+      <c r="I8" s="88">
         <v>999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="89">
+      <c r="B9" s="88">
+        <v>10</v>
+      </c>
+      <c r="C9" s="88">
+        <v>50</v>
+      </c>
+      <c r="D9" s="88">
+        <v>1</v>
+      </c>
+      <c r="E9" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="F9" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="H9" s="88">
+        <v>50</v>
+      </c>
+      <c r="I9" s="88">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="88">
         <v>20</v>
       </c>
-      <c r="C8" s="89">
-        <v>0</v>
-      </c>
-      <c r="D8" s="89">
+      <c r="C10" s="88">
+        <v>0</v>
+      </c>
+      <c r="D10" s="88">
         <v>1</v>
       </c>
-      <c r="E8" s="89">
+      <c r="E10" s="88">
         <v>0.03</v>
       </c>
-      <c r="F8" s="89">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G8" s="89">
+      <c r="F10" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="H10" s="88">
         <v>50</v>
       </c>
-      <c r="H8" s="89">
+      <c r="I10" s="88">
         <v>999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="89">
-        <v>10</v>
-      </c>
-      <c r="C9" s="89">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="88">
+        <v>20</v>
+      </c>
+      <c r="C11" s="88">
         <v>50</v>
       </c>
-      <c r="D9" s="89">
+      <c r="D11" s="88">
         <v>1</v>
       </c>
-      <c r="E9" s="89">
+      <c r="E11" s="88">
         <v>0.03</v>
       </c>
-      <c r="F9" s="89">
+      <c r="F11" s="88">
         <v>0.6</v>
       </c>
-      <c r="G9" s="89">
+      <c r="G11" s="88">
+        <v>0.6</v>
+      </c>
+      <c r="H11" s="88">
         <v>50</v>
       </c>
-      <c r="H9" s="89">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="79" t="s">
-        <v>161</v>
-      </c>
-      <c r="B10" s="89">
+      <c r="I11" s="88">
         <v>20</v>
       </c>
-      <c r="C10" s="89">
-        <v>0</v>
-      </c>
-      <c r="D10" s="89">
-        <v>1</v>
-      </c>
-      <c r="E10" s="89">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="79" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="88">
+        <v>20</v>
+      </c>
+      <c r="C12" s="88">
+        <v>50</v>
+      </c>
+      <c r="D12" s="88">
+        <v>2</v>
+      </c>
+      <c r="E12" s="88">
         <v>0.03</v>
       </c>
-      <c r="F10" s="89">
-        <v>0.6</v>
-      </c>
-      <c r="G10" s="89">
+      <c r="F12" s="88">
+        <v>0.7</v>
+      </c>
+      <c r="G12" s="88">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="88">
         <v>50</v>
       </c>
-      <c r="H10" s="89">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="89">
-        <v>20</v>
-      </c>
-      <c r="C11" s="89">
-        <v>50</v>
-      </c>
-      <c r="D11" s="89">
-        <v>1</v>
-      </c>
-      <c r="E11" s="89">
-        <v>0.03</v>
-      </c>
-      <c r="F11" s="89">
-        <v>0.6</v>
-      </c>
-      <c r="G11" s="89">
-        <v>50</v>
-      </c>
-      <c r="H11" s="89">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" s="89">
-        <v>20</v>
-      </c>
-      <c r="C12" s="89">
-        <v>50</v>
-      </c>
-      <c r="D12" s="89">
-        <v>2</v>
-      </c>
-      <c r="E12" s="89">
-        <v>0.03</v>
-      </c>
-      <c r="F12" s="89">
-        <v>0.7</v>
-      </c>
-      <c r="G12" s="89">
-        <v>50</v>
-      </c>
-      <c r="H12" s="89">
+      <c r="I12" s="88">
         <v>20</v>
       </c>
     </row>
@@ -12711,10 +12740,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -12788,7 +12817,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="18"/>
     </row>
@@ -12863,7 +12892,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -13127,7 +13156,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -13138,237 +13167,237 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="C6" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="D6" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="E6" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="F6" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="G6" s="79" t="s">
         <v>178</v>
-      </c>
-      <c r="G6" s="79" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="90">
+        <v>179</v>
+      </c>
+      <c r="B7" s="89">
         <v>40360</v>
       </c>
       <c r="C7" s="79">
         <v>30</v>
       </c>
-      <c r="D7" s="91">
-        <v>0</v>
-      </c>
-      <c r="E7" s="91">
-        <v>0</v>
-      </c>
-      <c r="F7" s="91">
+      <c r="D7" s="90">
+        <v>0</v>
+      </c>
+      <c r="E7" s="90">
+        <v>0</v>
+      </c>
+      <c r="F7" s="90">
         <v>25</v>
       </c>
-      <c r="G7" s="91">
+      <c r="G7" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="90">
+        <v>180</v>
+      </c>
+      <c r="B8" s="89">
         <v>40725</v>
       </c>
       <c r="C8" s="79">
         <v>30</v>
       </c>
-      <c r="D8" s="91">
-        <v>0</v>
-      </c>
-      <c r="E8" s="91">
-        <v>0</v>
-      </c>
-      <c r="F8" s="91">
+      <c r="D8" s="90">
+        <v>0</v>
+      </c>
+      <c r="E8" s="90">
+        <v>0</v>
+      </c>
+      <c r="F8" s="90">
         <v>26</v>
       </c>
-      <c r="G8" s="91">
+      <c r="G8" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="90">
+        <v>181</v>
+      </c>
+      <c r="B9" s="89">
         <v>40725</v>
       </c>
       <c r="C9" s="79">
         <v>15</v>
       </c>
-      <c r="D9" s="91">
-        <v>0</v>
-      </c>
-      <c r="E9" s="91">
-        <v>0</v>
-      </c>
-      <c r="F9" s="91">
+      <c r="D9" s="90">
+        <v>0</v>
+      </c>
+      <c r="E9" s="90">
+        <v>0</v>
+      </c>
+      <c r="F9" s="90">
         <v>11</v>
       </c>
-      <c r="G9" s="91">
+      <c r="G9" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" s="90">
+        <v>182</v>
+      </c>
+      <c r="B10" s="89">
         <v>40725</v>
       </c>
       <c r="C10" s="79">
         <v>15</v>
       </c>
-      <c r="D10" s="91">
-        <v>0</v>
-      </c>
-      <c r="E10" s="91">
-        <v>0</v>
-      </c>
-      <c r="F10" s="91">
+      <c r="D10" s="90">
+        <v>0</v>
+      </c>
+      <c r="E10" s="90">
+        <v>0</v>
+      </c>
+      <c r="F10" s="90">
         <v>11</v>
       </c>
-      <c r="G10" s="91">
+      <c r="G10" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="90">
+        <v>180</v>
+      </c>
+      <c r="B11" s="89">
         <v>41091</v>
       </c>
       <c r="C11" s="79">
         <v>30</v>
       </c>
-      <c r="D11" s="91">
-        <v>0</v>
-      </c>
-      <c r="E11" s="91">
-        <v>0</v>
-      </c>
-      <c r="F11" s="91">
+      <c r="D11" s="90">
+        <v>0</v>
+      </c>
+      <c r="E11" s="90">
+        <v>0</v>
+      </c>
+      <c r="F11" s="90">
         <v>27</v>
       </c>
-      <c r="G11" s="91">
+      <c r="G11" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="B12" s="90">
+        <v>180</v>
+      </c>
+      <c r="B12" s="89">
         <v>41456</v>
       </c>
       <c r="C12" s="79">
         <v>30</v>
       </c>
-      <c r="D12" s="91">
-        <v>0</v>
-      </c>
-      <c r="E12" s="91">
-        <v>0</v>
-      </c>
-      <c r="F12" s="91">
+      <c r="D12" s="90">
+        <v>0</v>
+      </c>
+      <c r="E12" s="90">
+        <v>0</v>
+      </c>
+      <c r="F12" s="90">
         <v>28</v>
       </c>
-      <c r="G12" s="91">
+      <c r="G12" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>184</v>
-      </c>
-      <c r="B13" s="90">
+        <v>183</v>
+      </c>
+      <c r="B13" s="89">
         <v>41821</v>
       </c>
       <c r="C13" s="79">
         <v>30</v>
       </c>
-      <c r="D13" s="91">
-        <v>0</v>
-      </c>
-      <c r="E13" s="91">
-        <v>0</v>
-      </c>
-      <c r="F13" s="91">
+      <c r="D13" s="90">
+        <v>0</v>
+      </c>
+      <c r="E13" s="90">
+        <v>0</v>
+      </c>
+      <c r="F13" s="90">
         <v>29</v>
       </c>
-      <c r="G13" s="91">
+      <c r="G13" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" s="90">
+        <v>183</v>
+      </c>
+      <c r="B14" s="89">
         <v>42186</v>
       </c>
       <c r="C14" s="79">
         <v>20</v>
       </c>
-      <c r="D14" s="91">
-        <v>0</v>
-      </c>
-      <c r="E14" s="91">
-        <v>0</v>
-      </c>
-      <c r="F14" s="91">
+      <c r="D14" s="90">
+        <v>0</v>
+      </c>
+      <c r="E14" s="90">
+        <v>0</v>
+      </c>
+      <c r="F14" s="90">
         <v>20</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="90">
+        <v>181</v>
+      </c>
+      <c r="B15" s="89">
         <v>42186</v>
       </c>
       <c r="C15" s="79">
         <v>20</v>
       </c>
-      <c r="D15" s="91">
-        <v>0</v>
-      </c>
-      <c r="E15" s="91">
-        <v>0</v>
-      </c>
-      <c r="F15" s="91">
+      <c r="D15" s="90">
+        <v>0</v>
+      </c>
+      <c r="E15" s="90">
+        <v>0</v>
+      </c>
+      <c r="F15" s="90">
         <v>20</v>
       </c>
-      <c r="G15" s="91">
+      <c r="G15" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E16" s="30"/>
       <c r="G16" s="30"/>
@@ -13462,15 +13491,15 @@
       <c r="A5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="104" t="s">
+      <c r="C5" s="106"/>
+      <c r="D5" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
       <c r="G5" s="42" t="s">
         <v>79</v>
       </c>
@@ -13493,10 +13522,10 @@
       <c r="E6" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="108"/>
+      <c r="G6" s="107"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
     </row>
@@ -13520,10 +13549,10 @@
       <c r="C9" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="105"/>
+      <c r="E9" s="104"/>
       <c r="F9" s="38" t="s">
         <v>64</v>
       </c>
@@ -13533,18 +13562,18 @@
     </row>
     <row r="10" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="108" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="109" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -13555,18 +13584,18 @@
       <c r="A12" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="107"/>
-      <c r="D12" s="105" t="s">
+      <c r="C12" s="106"/>
+      <c r="D12" s="104" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105" t="s">
+      <c r="E12" s="104"/>
+      <c r="F12" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="105"/>
+      <c r="G12" s="104"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>

</xml_diff>

<commit_message>
contingent annuity for disability benefits
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="2" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -1529,9 +1529,6 @@
     <t>r.vben</t>
   </si>
   <si>
-    <t>H12</t>
-  </si>
-  <si>
     <t>factor.ca</t>
   </si>
   <si>
@@ -1746,6 +1743,9 @@
   </si>
   <si>
     <t>factor.ca.disb</t>
+  </si>
+  <si>
+    <t>I12</t>
   </si>
 </sst>
 </file>
@@ -2252,17 +2252,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6673,7 +6673,7 @@
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="111"/>
       <c r="C6" s="111"/>
@@ -7237,7 +7237,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
@@ -7315,8 +7315,8 @@
       <c r="G5" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
-        <v>222</v>
+      <c r="A7" s="113" t="s">
+        <v>221</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>76</v>
@@ -7336,15 +7336,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="115"/>
-      <c r="B8" s="116" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="114" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -7384,7 +7384,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7593,7 +7593,7 @@
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>68</v>
@@ -7602,7 +7602,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>71</v>
@@ -7613,89 +7613,89 @@
     </row>
     <row r="4" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D4" s="101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G4" s="101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" s="101" t="s">
-        <v>213</v>
-      </c>
-      <c r="E5" s="113" t="s">
-        <v>216</v>
-      </c>
-      <c r="F5" s="113"/>
+        <v>212</v>
+      </c>
+      <c r="E5" s="115" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="115"/>
       <c r="G5" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="97" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" s="101" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="113" t="s">
-        <v>217</v>
-      </c>
-      <c r="F6" s="113"/>
+        <v>216</v>
+      </c>
+      <c r="E6" s="115" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="115"/>
       <c r="G6" s="101" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H6" s="101" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" s="101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="101" t="s">
-        <v>214</v>
-      </c>
-      <c r="E7" s="113" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="113"/>
+        <v>213</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="115"/>
       <c r="G7" s="101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H7" s="101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7822,95 +7822,95 @@
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="J5" s="114" t="s">
-        <v>188</v>
-      </c>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114" t="s">
-        <v>201</v>
-      </c>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114"/>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114"/>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114"/>
+      <c r="J5" s="116" t="s">
+        <v>187</v>
+      </c>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116" t="s">
+        <v>200</v>
+      </c>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>97</v>
       </c>
       <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" t="s">
         <v>194</v>
       </c>
-      <c r="D6" t="s">
-        <v>195</v>
-      </c>
       <c r="E6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" t="s">
         <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="J6" s="93" t="s">
+      <c r="K6" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="K6" s="93" t="s">
+      <c r="L6" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="L6" s="93" t="s">
+      <c r="M6" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="M6" s="93" t="s">
-        <v>193</v>
-      </c>
       <c r="N6" s="93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O6" s="93" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" s="93" t="s">
         <v>199</v>
       </c>
-      <c r="P6" s="93" t="s">
-        <v>200</v>
-      </c>
       <c r="Q6" s="95" t="s">
+        <v>189</v>
+      </c>
+      <c r="R6" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="R6" s="95" t="s">
+      <c r="S6" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="S6" s="95" t="s">
+      <c r="T6" s="95" t="s">
         <v>192</v>
       </c>
-      <c r="T6" s="95" t="s">
-        <v>193</v>
-      </c>
       <c r="U6" s="95" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="V6" s="95" t="s">
+        <v>198</v>
+      </c>
+      <c r="W6" s="95" t="s">
         <v>199</v>
-      </c>
-      <c r="W6" s="95" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
@@ -12435,7 +12435,7 @@
     </row>
     <row r="108" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N108" s="92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O108">
         <f>SUM(O42:O106)</f>
@@ -12446,7 +12446,7 @@
         <v>80.573925783148752</v>
       </c>
       <c r="U108" s="92" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V108">
         <f>SUM(V42:V106)</f>
@@ -12481,8 +12481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12508,7 +12508,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>169</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -12528,10 +12528,10 @@
         <v>166</v>
       </c>
       <c r="F6" s="88" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H6" s="88" t="s">
         <v>168</v>
@@ -13156,7 +13156,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -13167,30 +13167,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="C6" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="D6" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="E6" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="F6" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="G6" s="79" t="s">
         <v>177</v>
-      </c>
-      <c r="G6" s="79" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="89">
         <v>40360</v>
@@ -13213,7 +13213,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="89">
         <v>40725</v>
@@ -13236,7 +13236,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="89">
         <v>40725</v>
@@ -13259,7 +13259,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="89">
         <v>40725</v>
@@ -13282,7 +13282,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="89">
         <v>41091</v>
@@ -13305,7 +13305,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="89">
         <v>41456</v>
@@ -13328,7 +13328,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" s="89">
         <v>41821</v>
@@ -13351,7 +13351,7 @@
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="89">
         <v>42186</v>
@@ -13374,7 +13374,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="89">
         <v>42186</v>
@@ -13397,7 +13397,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E16" s="30"/>
       <c r="G16" s="30"/>

</xml_diff>

<commit_message>
tier dependent EEC rate
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="227">
   <si>
     <t>Notes</t>
   </si>
@@ -1298,6 +1298,381 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">No vestinguntil retirement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No active members, do not need to model </t>
+  </si>
+  <si>
+    <t>Benefit
+AV2015 pdf p79, p92
+CAFR2015, p126</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Only 22 older members in 2015, will not model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Need to evaluate if the death benefits are worth modeling. 
+ - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Refund of contribution with interest. 
+ - limited pension for qualified survivor. </t>
+    </r>
+  </si>
+  <si>
+    <t>Return of contribution</t>
+  </si>
+  <si>
+    <t>No refund</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">refund contribution with interest
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Do not model for now)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">refund contribution with interest
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Do not model for now)</t>
+    </r>
+  </si>
+  <si>
+    <t>Healthy mortality table is used for disabled?</t>
+  </si>
+  <si>
+    <t>qxt.fire.yos</t>
+  </si>
+  <si>
+    <t>qxt.plc.yos</t>
+  </si>
+  <si>
+    <t>qxt.fire.age</t>
+  </si>
+  <si>
+    <t>qxt.plc.age</t>
+  </si>
+  <si>
+    <t>Modeling of contingent annuity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeled as 60% contingent annuity for tier 3, 4, 5
+Modeled as 70% contingent annuity for tier 6. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeled as 100% contingent annuity
+Notes: 
+1. Tier 1 is so small that the approximation would not have a big impact on over results. 
+2. For Tier 2, it requires 25 yos for the benefit factor to be greater than 50%. The average retirement age is around 50, so there may not be a great number of retirees whose benefit factors are greater than 50%.  
+</t>
+  </si>
+  <si>
+    <t>tier</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>r.yos</t>
+  </si>
+  <si>
+    <t>r.age</t>
+  </si>
+  <si>
+    <t>fasyears</t>
+  </si>
+  <si>
+    <t>cola</t>
+  </si>
+  <si>
+    <t>v.yos</t>
+  </si>
+  <si>
+    <t>r.vben</t>
+  </si>
+  <si>
+    <t>factor.ca</t>
+  </si>
+  <si>
+    <r>
+      <t>Question: 
+  - (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOLVED</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) No vested term for Tier 1, 2, 4?(SOLVED, do not need to model 1,2, no vesting for 4)
+  - Are the term benefits life annuity or contingent annuity? (Currently modeld as life annuity)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Date Established</t>
+  </si>
+  <si>
+    <t>Initial Years</t>
+  </si>
+  <si>
+    <t>Initial Amount</t>
+  </si>
+  <si>
+    <t>Annual Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years remaining </t>
+  </si>
+  <si>
+    <t>Outstanding Balance</t>
+  </si>
+  <si>
+    <t>Actuarial Loss**</t>
+  </si>
+  <si>
+    <t>Actuarial Loss</t>
+  </si>
+  <si>
+    <t>Change in Assumptions</t>
+  </si>
+  <si>
+    <t>Plan Amendment</t>
+  </si>
+  <si>
+    <t>Actuarial Gain</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>G15</t>
+  </si>
+  <si>
+    <t>fas</t>
+  </si>
+  <si>
+    <t>salary(fas)</t>
+  </si>
+  <si>
+    <t>Retire at age55</t>
+  </si>
+  <si>
+    <t>Bx</t>
+  </si>
+  <si>
+    <t>DROP pay</t>
+  </si>
+  <si>
+    <t>DROP account</t>
+  </si>
+  <si>
+    <t>DROP cash flow</t>
+  </si>
+  <si>
+    <t>la cash flow</t>
+  </si>
+  <si>
+    <t>qxm</t>
+  </si>
+  <si>
+    <t>survival</t>
+  </si>
+  <si>
+    <t>Disc Rate</t>
+  </si>
+  <si>
+    <t>Disc factor</t>
+  </si>
+  <si>
+    <t>PV at 55</t>
+  </si>
+  <si>
+    <t>DROP cf disc</t>
+  </si>
+  <si>
+    <t>la cf disc</t>
+  </si>
+  <si>
+    <t>Retire at age65</t>
+  </si>
+  <si>
+    <t>PV at 65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eligibility </t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>Eligible for Service retirement</t>
+  </si>
+  <si>
+    <t>Service connected</t>
+  </si>
+  <si>
+    <t>yos &gt;=20</t>
+  </si>
+  <si>
+    <t>100% accrued retirement benefit
+Not to sceed 50% Normal pension base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% of normal pension base </t>
+  </si>
+  <si>
+    <t>yos&gt;=20</t>
+  </si>
+  <si>
+    <t>100% accrued retirement benefit
+Not to sceed 55% Normal pension base</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">55% of Normal pension base if yos &gt;=25, otherwise 50% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(only need to model 55%)</t>
+    </r>
+  </si>
+  <si>
+    <t>yos&gt;=10</t>
+  </si>
+  <si>
+    <t>80% accrued retirement benefit
+Not to sceed 40% Normal pension base</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>75% of FAS</t>
+  </si>
+  <si>
+    <t>For former Tier 2: 100% accrued benefit, not to exceed 55% of NPB
+For others: 40% of FAS</t>
+  </si>
+  <si>
+    <t>80% of FAS</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death after retirement
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeling:
+- assuming all disabilities  are service connceted.
+- QSSs' benefits are modeled as a fixed proportion of the pension received by the deceased member immediately preceding the date of death.
+   - Tier 1: 80%  
+   - Tier 2: 80%
+   - Tier 3/4: 60%
+   - Tier 5:  60%
+   - Tier 6: 80% </t>
+  </si>
+  <si>
+    <t>factor.ca.disb</t>
+  </si>
+  <si>
     <r>
       <t>Tier 1:
  - Normal contribution rate 6%
@@ -1351,7 +1726,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>exempt if yos&gt;=33</t>
+      <t>exempt if yos&gt;33</t>
     </r>
     <r>
       <rPr>
@@ -1364,388 +1739,19 @@
       <t xml:space="preserve">
 Tier 6
  - Normal contribuiton rate 11%
- - 9% if yos&gt;=25 (plus 2% of the 11% to support health benefit, exempt if yos &gt; 25)
- - exempt if yos &gt;= 33 
+ - 2% of the 11% to support health benefit, exempt if yos &gt; 25
+ - exempt if yos &gt;=33 
 (See CAFR 2015 p124)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">No vestinguntil retirement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No active members, do not need to model </t>
-  </si>
-  <si>
-    <t>Benefit
-AV2015 pdf p79, p92
-CAFR2015, p126</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Only 22 older members in 2015, will not model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Need to evaluate if the death benefits are worth modeling. 
- - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Refund of contribution with interest. 
- - limited pension for qualified survivor. </t>
-    </r>
-  </si>
-  <si>
-    <t>Return of contribution</t>
-  </si>
-  <si>
-    <t>No refund</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">refund contribution with interest
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-(Do not model for now)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">refund contribution with interest
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-(Do not model for now)</t>
-    </r>
-  </si>
-  <si>
-    <t>Healthy mortality table is used for disabled?</t>
-  </si>
-  <si>
-    <t>qxt.fire.yos</t>
-  </si>
-  <si>
-    <t>qxt.plc.yos</t>
-  </si>
-  <si>
-    <t>qxt.fire.age</t>
-  </si>
-  <si>
-    <t>qxt.plc.age</t>
-  </si>
-  <si>
-    <t>Modeling of contingent annuity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modeled as 60% contingent annuity for tier 3, 4, 5
-Modeled as 70% contingent annuity for tier 6. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modeled as 100% contingent annuity
-Notes: 
-1. Tier 1 is so small that the approximation would not have a big impact on over results. 
-2. For Tier 2, it requires 25 yos for the benefit factor to be greater than 50%. The average retirement age is around 50, so there may not be a great number of retirees whose benefit factors are greater than 50%.  
-</t>
-  </si>
-  <si>
-    <t>tier</t>
-  </si>
-  <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>t3</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>r.yos</t>
-  </si>
-  <si>
-    <t>r.age</t>
-  </si>
-  <si>
-    <t>fasyears</t>
-  </si>
-  <si>
-    <t>cola</t>
-  </si>
-  <si>
-    <t>v.yos</t>
-  </si>
-  <si>
-    <t>r.vben</t>
-  </si>
-  <si>
-    <t>factor.ca</t>
-  </si>
-  <si>
-    <r>
-      <t>Question: 
-  - (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SOLVED</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) No vested term for Tier 1, 2, 4?(SOLVED, do not need to model 1,2, no vesting for 4)
-  - Are the term benefits life annuity or contingent annuity? (Currently modeld as life annuity)
-</t>
-    </r>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Date Established</t>
-  </si>
-  <si>
-    <t>Initial Years</t>
-  </si>
-  <si>
-    <t>Initial Amount</t>
-  </si>
-  <si>
-    <t>Annual Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years remaining </t>
-  </si>
-  <si>
-    <t>Outstanding Balance</t>
-  </si>
-  <si>
-    <t>Actuarial Loss**</t>
-  </si>
-  <si>
-    <t>Actuarial Loss</t>
-  </si>
-  <si>
-    <t>Change in Assumptions</t>
-  </si>
-  <si>
-    <t>Plan Amendment</t>
-  </si>
-  <si>
-    <t>Actuarial Gain</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>G15</t>
-  </si>
-  <si>
-    <t>fas</t>
-  </si>
-  <si>
-    <t>salary(fas)</t>
-  </si>
-  <si>
-    <t>Retire at age55</t>
-  </si>
-  <si>
-    <t>Bx</t>
-  </si>
-  <si>
-    <t>DROP pay</t>
-  </si>
-  <si>
-    <t>DROP account</t>
-  </si>
-  <si>
-    <t>DROP cash flow</t>
-  </si>
-  <si>
-    <t>la cash flow</t>
-  </si>
-  <si>
-    <t>qxm</t>
-  </si>
-  <si>
-    <t>survival</t>
-  </si>
-  <si>
-    <t>Disc Rate</t>
-  </si>
-  <si>
-    <t>Disc factor</t>
-  </si>
-  <si>
-    <t>PV at 55</t>
-  </si>
-  <si>
-    <t>DROP cf disc</t>
-  </si>
-  <si>
-    <t>la cf disc</t>
-  </si>
-  <si>
-    <t>Retire at age65</t>
-  </si>
-  <si>
-    <t>PV at 65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eligibility </t>
-  </si>
-  <si>
-    <t>Benefit</t>
-  </si>
-  <si>
-    <t>Eligible for Service retirement</t>
-  </si>
-  <si>
-    <t>Service connected</t>
-  </si>
-  <si>
-    <t>yos &gt;=20</t>
-  </si>
-  <si>
-    <t>100% accrued retirement benefit
-Not to sceed 50% Normal pension base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50% of normal pension base </t>
-  </si>
-  <si>
-    <t>yos&gt;=20</t>
-  </si>
-  <si>
-    <t>100% accrued retirement benefit
-Not to sceed 55% Normal pension base</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">55% of Normal pension base if yos &gt;=25, otherwise 50% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(only need to model 55%)</t>
-    </r>
-  </si>
-  <si>
-    <t>yos&gt;=10</t>
-  </si>
-  <si>
-    <t>80% accrued retirement benefit
-Not to sceed 40% Normal pension base</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>75% of FAS</t>
-  </si>
-  <si>
-    <t>For former Tier 2: 100% accrued benefit, not to exceed 55% of NPB
-For others: 40% of FAS</t>
-  </si>
-  <si>
-    <t>80% of FAS</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death after retirement
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modeling:
-- assuming all disabilities  are service connceted.
-- QSSs' benefits are modeled as a fixed proportion of the pension received by the deceased member immediately preceding the date of death.
-   - Tier 1: 80%  
-   - Tier 2: 80%
-   - Tier 3/4: 60%
-   - Tier 5:  60%
-   - Tier 6: 80% </t>
-  </si>
-  <si>
-    <t>factor.ca.disb</t>
-  </si>
-  <si>
-    <t>I12</t>
+    <t>EEC.exempt.yos</t>
+  </si>
+  <si>
+    <t>EEC.rate</t>
+  </si>
+  <si>
+    <t>K12</t>
   </si>
 </sst>
 </file>
@@ -6631,19 +6637,19 @@
     </row>
     <row r="4" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="B4" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="D4" s="76" t="s">
         <v>123</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="104" t="s">
         <v>124</v>
@@ -6652,28 +6658,28 @@
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="76" t="s">
+      <c r="F5" s="104" t="s">
         <v>146</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="104" t="s">
-        <v>147</v>
       </c>
       <c r="G5" s="104"/>
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="111"/>
       <c r="C6" s="111"/>
@@ -6783,10 +6789,10 @@
         <v>85</v>
       </c>
       <c r="B5" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="79" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7023,10 +7029,10 @@
         <v>97</v>
       </c>
       <c r="B5" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="79" t="s">
         <v>151</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7238,7 +7244,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7316,7 +7322,7 @@
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="113" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>76</v>
@@ -7338,7 +7344,7 @@
     <row r="8" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="113"/>
       <c r="B8" s="114" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="114"/>
       <c r="D8" s="114"/>
@@ -7593,7 +7599,7 @@
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>68</v>
@@ -7602,7 +7608,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>71</v>
@@ -7613,89 +7619,89 @@
     </row>
     <row r="4" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="101" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E4" s="101" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G4" s="101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" s="101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5" s="101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F5" s="115"/>
       <c r="G5" s="101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" s="101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" s="101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" s="101" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D7" s="101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="115"/>
       <c r="G7" s="101" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H7" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7714,7 +7720,7 @@
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" s="99"/>
       <c r="E9" s="99"/>
@@ -7777,7 +7783,7 @@
     <row r="5" spans="1:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7822,7 +7828,7 @@
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2">
         <v>7.4999999999999997E-2</v>
@@ -7830,7 +7836,7 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J5" s="116" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K5" s="116"/>
       <c r="L5" s="116"/>
@@ -7839,7 +7845,7 @@
       <c r="O5" s="116"/>
       <c r="P5" s="116"/>
       <c r="Q5" s="116" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R5" s="116"/>
       <c r="S5" s="116"/>
@@ -7853,64 +7859,64 @@
         <v>97</v>
       </c>
       <c r="C6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" t="s">
         <v>193</v>
       </c>
-      <c r="D6" t="s">
-        <v>194</v>
-      </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" t="s">
         <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J6" s="93" t="s">
         <v>188</v>
       </c>
-      <c r="J6" s="93" t="s">
+      <c r="K6" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="K6" s="93" t="s">
+      <c r="L6" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="L6" s="93" t="s">
+      <c r="M6" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="M6" s="93" t="s">
-        <v>192</v>
-      </c>
       <c r="N6" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O6" s="93" t="s">
+        <v>197</v>
+      </c>
+      <c r="P6" s="93" t="s">
         <v>198</v>
       </c>
-      <c r="P6" s="93" t="s">
-        <v>199</v>
-      </c>
       <c r="Q6" s="95" t="s">
+        <v>188</v>
+      </c>
+      <c r="R6" s="95" t="s">
         <v>189</v>
       </c>
-      <c r="R6" s="95" t="s">
+      <c r="S6" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="S6" s="95" t="s">
+      <c r="T6" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="T6" s="95" t="s">
-        <v>192</v>
-      </c>
       <c r="U6" s="95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="V6" s="95" t="s">
+        <v>197</v>
+      </c>
+      <c r="W6" s="95" t="s">
         <v>198</v>
-      </c>
-      <c r="W6" s="95" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
@@ -12435,7 +12441,7 @@
     </row>
     <row r="108" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N108" s="92" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O108">
         <f>SUM(O42:O106)</f>
@@ -12446,7 +12452,7 @@
         <v>80.573925783148752</v>
       </c>
       <c r="U108" s="92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="V108">
         <f>SUM(V42:V106)</f>
@@ -12479,23 +12485,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>87</v>
       </c>
@@ -12503,46 +12510,52 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" s="88" t="s">
+        <v>166</v>
+      </c>
+      <c r="J6" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="K6" s="88" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
         <v>156</v>
-      </c>
-      <c r="B6" s="88" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="88" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="88" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="88" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" s="88" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6" s="88" t="s">
-        <v>223</v>
-      </c>
-      <c r="H6" s="88" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="88" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
-        <v>157</v>
       </c>
       <c r="B7" s="88">
         <v>20</v>
@@ -12568,10 +12581,16 @@
       <c r="I7" s="88">
         <v>999</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="88">
+        <v>0.06</v>
+      </c>
+      <c r="K7" s="88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="88">
         <v>20</v>
@@ -12597,10 +12616,16 @@
       <c r="I8" s="88">
         <v>999</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="88">
+        <v>0.06</v>
+      </c>
+      <c r="K8" s="88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="88">
         <v>10</v>
@@ -12626,10 +12651,16 @@
       <c r="I9" s="88">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="88">
+        <v>0.08</v>
+      </c>
+      <c r="K9" s="88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" s="88">
         <v>20</v>
@@ -12655,10 +12686,16 @@
       <c r="I10" s="88">
         <v>999</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="88">
+        <v>0.08</v>
+      </c>
+      <c r="K10" s="88">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="88">
         <v>20</v>
@@ -12684,10 +12721,16 @@
       <c r="I11" s="88">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="88">
+        <v>0.09</v>
+      </c>
+      <c r="K11" s="88">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="88">
         <v>20</v>
@@ -12712,6 +12755,12 @@
       </c>
       <c r="I12" s="88">
         <v>20</v>
+      </c>
+      <c r="J12" s="88">
+        <v>0.11</v>
+      </c>
+      <c r="K12" s="88">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -12761,8 +12810,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12817,7 +12866,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C8" s="18"/>
     </row>
@@ -13156,7 +13205,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -13167,30 +13216,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="C6" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="D6" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="E6" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="F6" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="G6" s="79" t="s">
         <v>176</v>
-      </c>
-      <c r="G6" s="79" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="89">
         <v>40360</v>
@@ -13213,7 +13262,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="89">
         <v>40725</v>
@@ -13236,7 +13285,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="89">
         <v>40725</v>
@@ -13259,7 +13308,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="89">
         <v>40725</v>
@@ -13282,7 +13331,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="89">
         <v>41091</v>
@@ -13305,7 +13354,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="89">
         <v>41456</v>
@@ -13328,7 +13377,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="89">
         <v>41821</v>
@@ -13351,7 +13400,7 @@
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" s="89">
         <v>42186</v>
@@ -13374,7 +13423,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="89">
         <v>42186</v>
@@ -13397,7 +13446,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E16" s="30"/>
       <c r="G16" s="30"/>
@@ -13562,14 +13611,14 @@
     </row>
     <row r="10" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="108"/>
       <c r="D10" s="108" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="108"/>
       <c r="F10" s="108"/>

</xml_diff>

<commit_message>
update cash flow comparison
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="15" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="Death_sum" sheetId="17" r:id="rId18"/>
     <sheet name="Death_dec" sheetId="5" r:id="rId19"/>
     <sheet name="DROP cashflow" sheetId="25" r:id="rId20"/>
-    <sheet name="Sheet1" sheetId="26" r:id="rId21"/>
+    <sheet name="GASB_cashflow" sheetId="26" r:id="rId21"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="267">
   <si>
     <t>Notes</t>
   </si>
@@ -2014,6 +2014,260 @@
 In the model, the deferred returns must be adjusted so that the total deferred return is equal to the difference between the initial AA and MA.
 Only effective when modeling all tiers together.</t>
   </si>
+  <si>
+    <t>G31</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Year
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Beginning
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>July 1,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Projected Beginning
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Plan Fiduciary
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Net Position
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(a)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Projected
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Total
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Contributions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(b)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Projected
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Benefit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Payments
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(c)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Projected
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Administrative
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expenses
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(d)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Projected
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Investment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Earnings
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(e)</t>
+    </r>
+  </si>
+  <si>
+    <t>MA.GASB</t>
+  </si>
+  <si>
+    <t>C.GASB</t>
+  </si>
+  <si>
+    <t>B.GASB</t>
+  </si>
+  <si>
+    <t>AdminExp.GASB</t>
+  </si>
+  <si>
+    <t>InvIncome.GASB</t>
+  </si>
 </sst>
 </file>
 
@@ -2025,7 +2279,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2178,6 +2432,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2249,7 +2514,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2562,6 +2827,21 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2604,20 +2884,50 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4290,15 +4600,15 @@
       <c r="A5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="124" t="s">
+      <c r="C5" s="132"/>
+      <c r="D5" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
       <c r="G5" s="42" t="s">
         <v>79</v>
       </c>
@@ -4321,10 +4631,10 @@
       <c r="E6" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="128" t="s">
+      <c r="F6" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="128"/>
+      <c r="G6" s="133"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
     </row>
@@ -4348,10 +4658,10 @@
       <c r="C9" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="130" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="125"/>
+      <c r="E9" s="130"/>
       <c r="F9" s="38" t="s">
         <v>64</v>
       </c>
@@ -4363,16 +4673,16 @@
       <c r="A10" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="134" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129" t="s">
+      <c r="C10" s="134"/>
+      <c r="D10" s="134" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -4383,18 +4693,18 @@
       <c r="A12" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="127"/>
-      <c r="D12" s="125" t="s">
+      <c r="C12" s="132"/>
+      <c r="D12" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125" t="s">
+      <c r="E12" s="130"/>
+      <c r="F12" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="125"/>
+      <c r="G12" s="130"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
@@ -4564,22 +4874,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="136" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131" t="s">
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
@@ -7301,10 +7611,10 @@
       <c r="E4" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="130" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="127"/>
+      <c r="G4" s="132"/>
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
@@ -7322,21 +7632,21 @@
       <c r="E5" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="125" t="s">
+      <c r="F5" s="130" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="125"/>
+      <c r="G5" s="130"/>
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="132" t="s">
+      <c r="A6" s="137" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -7948,30 +8258,30 @@
       <c r="A4" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="138" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
     </row>
     <row r="5" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="131" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134" t="s">
+      <c r="A7" s="139" t="s">
         <v>206</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -7980,10 +8290,10 @@
       <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="130" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="127"/>
+      <c r="E7" s="132"/>
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
@@ -7992,15 +8302,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="134"/>
-      <c r="B8" s="135" t="s">
+      <c r="A8" s="139"/>
+      <c r="B8" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="140"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -8300,10 +8610,10 @@
       <c r="D5" s="99" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="136" t="s">
+      <c r="E5" s="141" t="s">
         <v>200</v>
       </c>
-      <c r="F5" s="136"/>
+      <c r="F5" s="141"/>
       <c r="G5" s="99" t="s">
         <v>203</v>
       </c>
@@ -8321,10 +8631,10 @@
       <c r="D6" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="136" t="s">
+      <c r="E6" s="141" t="s">
         <v>201</v>
       </c>
-      <c r="F6" s="136"/>
+      <c r="F6" s="141"/>
       <c r="G6" s="99" t="s">
         <v>201</v>
       </c>
@@ -8343,10 +8653,10 @@
       <c r="D7" s="99" t="s">
         <v>198</v>
       </c>
-      <c r="E7" s="136" t="s">
+      <c r="E7" s="141" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="136"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="99" t="s">
         <v>202</v>
       </c>
@@ -8773,24 +9083,24 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="J5" s="137" t="s">
+      <c r="J5" s="142" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
-      <c r="O5" s="137"/>
-      <c r="P5" s="137"/>
-      <c r="Q5" s="137" t="s">
+      <c r="K5" s="142"/>
+      <c r="L5" s="142"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="142"/>
+      <c r="Q5" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="R5" s="137"/>
-      <c r="S5" s="137"/>
-      <c r="T5" s="137"/>
-      <c r="U5" s="137"/>
-      <c r="V5" s="137"/>
-      <c r="W5" s="137"/>
+      <c r="R5" s="142"/>
+      <c r="S5" s="142"/>
+      <c r="T5" s="142"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="142"/>
+      <c r="W5" s="142"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -13423,10 +13733,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13434,157 +13744,571 @@
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="143" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="144" t="s">
+        <v>257</v>
+      </c>
+      <c r="D5" s="144" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5" s="144" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="144" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="144" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="145" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="146" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="146" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="146" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" s="146" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="146" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="147">
+        <v>2014</v>
+      </c>
+      <c r="C7" s="148">
         <v>16990</v>
       </c>
-      <c r="B2">
+      <c r="D7" s="149">
         <v>607</v>
       </c>
-      <c r="C2">
+      <c r="E7" s="148">
         <v>919</v>
       </c>
-      <c r="D2">
-        <f>100*(B2-C2)/A2</f>
-        <v>-1.8363743378457917</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F7" s="149">
+        <v>18</v>
+      </c>
+      <c r="G7" s="148">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="150">
+        <v>2015</v>
+      </c>
+      <c r="C8" s="151">
         <v>17347</v>
       </c>
-      <c r="B3">
+      <c r="D8" s="152">
         <v>632</v>
       </c>
-      <c r="C3">
+      <c r="E8" s="151">
         <v>970</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">100*(B3-C3)/A3</f>
-        <v>-1.9484637113045484</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F8" s="152">
+        <v>13</v>
+      </c>
+      <c r="G8" s="151">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="150">
+        <v>2016</v>
+      </c>
+      <c r="C9" s="151">
         <v>18302</v>
       </c>
-      <c r="B4">
+      <c r="D9" s="152">
         <v>634</v>
       </c>
-      <c r="C4">
+      <c r="E9" s="151">
         <v>1104</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>-2.5680253524205003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F9" s="152">
+        <v>13</v>
+      </c>
+      <c r="G9" s="151">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="150">
+        <v>2017</v>
+      </c>
+      <c r="C10" s="151">
         <v>19190</v>
       </c>
-      <c r="B5">
+      <c r="D10" s="152">
         <v>609</v>
       </c>
-      <c r="C5">
+      <c r="E10" s="151">
         <v>1050</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-2.2980719124544033</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F10" s="152">
+        <v>13</v>
+      </c>
+      <c r="G10" s="151">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="150">
+        <v>2018</v>
+      </c>
+      <c r="C11" s="151">
         <v>20176</v>
       </c>
-      <c r="B6">
+      <c r="D11" s="152">
         <v>616</v>
       </c>
-      <c r="C6">
+      <c r="E11" s="151">
         <v>1149</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-2.6417525773195876</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F11" s="152">
+        <v>13</v>
+      </c>
+      <c r="G11" s="151">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="150">
+        <v>2019</v>
+      </c>
+      <c r="C12" s="151">
         <v>21139</v>
       </c>
-      <c r="B7">
+      <c r="D12" s="152">
         <v>586</v>
       </c>
-      <c r="C7">
+      <c r="E12" s="151">
         <v>1267</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-3.2215336581673686</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F12" s="152">
+        <v>12</v>
+      </c>
+      <c r="G12" s="151">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="150">
+        <v>2020</v>
+      </c>
+      <c r="C13" s="151">
         <v>22019</v>
       </c>
-      <c r="B8">
+      <c r="D13" s="152">
         <v>538</v>
       </c>
-      <c r="C8">
+      <c r="E13" s="151">
         <v>1212</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>-3.0609927789636222</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F13" s="152">
+        <v>12</v>
+      </c>
+      <c r="G13" s="151">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="150">
+        <v>2021</v>
+      </c>
+      <c r="C14" s="151">
         <v>22971</v>
       </c>
-      <c r="B9">
+      <c r="D14" s="152">
         <v>537</v>
       </c>
-      <c r="C9">
+      <c r="E14" s="151">
         <v>1283</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>-3.2475730268599539</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>32920</v>
-      </c>
-      <c r="B10">
+      <c r="F14" s="152">
+        <v>12</v>
+      </c>
+      <c r="G14" s="151">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="150">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="151">
+        <v>23920</v>
+      </c>
+      <c r="D15" s="152">
         <v>538</v>
       </c>
-      <c r="C10">
+      <c r="E15" s="151">
         <v>1350</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>-2.4665856622114215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="F15" s="152">
+        <v>12</v>
+      </c>
+      <c r="G15" s="151">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="153">
+        <v>2023</v>
+      </c>
+      <c r="C16" s="154">
         <v>24871</v>
       </c>
-      <c r="B11">
+      <c r="D16" s="155">
         <v>539</v>
       </c>
-      <c r="C11">
+      <c r="E16" s="154">
         <v>1416</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-3.5261951670620402</v>
+      <c r="F16" s="155">
+        <v>12</v>
+      </c>
+      <c r="G16" s="154">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="150">
+        <v>2038</v>
+      </c>
+      <c r="C17" s="151">
+        <v>32905</v>
+      </c>
+      <c r="D17" s="152">
+        <v>197</v>
+      </c>
+      <c r="E17" s="151">
+        <v>2584</v>
+      </c>
+      <c r="F17" s="152">
+        <v>5</v>
+      </c>
+      <c r="G17" s="151">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="150">
+        <v>2039</v>
+      </c>
+      <c r="C18" s="151">
+        <v>32883</v>
+      </c>
+      <c r="D18" s="152">
+        <v>214</v>
+      </c>
+      <c r="E18" s="151">
+        <v>2667</v>
+      </c>
+      <c r="F18" s="152">
+        <v>4</v>
+      </c>
+      <c r="G18" s="151">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="150">
+        <v>2040</v>
+      </c>
+      <c r="C19" s="151">
+        <v>32791</v>
+      </c>
+      <c r="D19" s="152">
+        <v>174</v>
+      </c>
+      <c r="E19" s="151">
+        <v>2734</v>
+      </c>
+      <c r="F19" s="152">
+        <v>4</v>
+      </c>
+      <c r="G19" s="151">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="150">
+        <v>2041</v>
+      </c>
+      <c r="C20" s="151">
+        <v>32581</v>
+      </c>
+      <c r="D20" s="152">
+        <v>91</v>
+      </c>
+      <c r="E20" s="151">
+        <v>2785</v>
+      </c>
+      <c r="F20" s="152">
+        <v>3</v>
+      </c>
+      <c r="G20" s="151">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="153">
+        <v>2042</v>
+      </c>
+      <c r="C21" s="154">
+        <v>32213</v>
+      </c>
+      <c r="D21" s="155">
+        <v>74</v>
+      </c>
+      <c r="E21" s="154">
+        <v>2824</v>
+      </c>
+      <c r="F21" s="155">
+        <v>2</v>
+      </c>
+      <c r="G21" s="154">
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="150">
+        <v>2082</v>
+      </c>
+      <c r="C22" s="151">
+        <v>1097</v>
+      </c>
+      <c r="D22" s="152">
+        <v>0</v>
+      </c>
+      <c r="E22" s="151">
+        <v>290</v>
+      </c>
+      <c r="F22" s="152">
+        <v>0</v>
+      </c>
+      <c r="G22" s="151">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="150">
+        <v>2083</v>
+      </c>
+      <c r="C23" s="151">
+        <v>877</v>
+      </c>
+      <c r="D23" s="152">
+        <v>0</v>
+      </c>
+      <c r="E23" s="151">
+        <v>239</v>
+      </c>
+      <c r="F23" s="152">
+        <v>0</v>
+      </c>
+      <c r="G23" s="151">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="150">
+        <v>2084</v>
+      </c>
+      <c r="C24" s="151">
+        <v>694</v>
+      </c>
+      <c r="D24" s="152">
+        <v>0</v>
+      </c>
+      <c r="E24" s="151">
+        <v>194</v>
+      </c>
+      <c r="F24" s="152">
+        <v>0</v>
+      </c>
+      <c r="G24" s="151">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="150">
+        <v>2085</v>
+      </c>
+      <c r="C25" s="151">
+        <v>543</v>
+      </c>
+      <c r="D25" s="152">
+        <v>0</v>
+      </c>
+      <c r="E25" s="151">
+        <v>156</v>
+      </c>
+      <c r="F25" s="152">
+        <v>0</v>
+      </c>
+      <c r="G25" s="151">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="153">
+        <v>2086</v>
+      </c>
+      <c r="C26" s="154">
+        <v>420</v>
+      </c>
+      <c r="D26" s="155">
+        <v>0</v>
+      </c>
+      <c r="E26" s="154">
+        <v>124</v>
+      </c>
+      <c r="F26" s="155">
+        <v>0</v>
+      </c>
+      <c r="G26" s="154">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="150">
+        <v>2101</v>
+      </c>
+      <c r="C27" s="151">
+        <v>2</v>
+      </c>
+      <c r="D27" s="152">
+        <v>0</v>
+      </c>
+      <c r="E27" s="151">
+        <v>1</v>
+      </c>
+      <c r="F27" s="152">
+        <v>0</v>
+      </c>
+      <c r="G27" s="151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="150">
+        <v>2102</v>
+      </c>
+      <c r="C28" s="151">
+        <v>2</v>
+      </c>
+      <c r="D28" s="152">
+        <v>0</v>
+      </c>
+      <c r="E28" s="151">
+        <v>1</v>
+      </c>
+      <c r="F28" s="152">
+        <v>0</v>
+      </c>
+      <c r="G28" s="151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="153">
+        <v>2103</v>
+      </c>
+      <c r="C29" s="154">
+        <v>1</v>
+      </c>
+      <c r="D29" s="155">
+        <v>0</v>
+      </c>
+      <c r="E29" s="154">
+        <v>0</v>
+      </c>
+      <c r="F29" s="155">
+        <v>0</v>
+      </c>
+      <c r="G29" s="154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="150">
+        <v>2115</v>
+      </c>
+      <c r="C30" s="151">
+        <v>0</v>
+      </c>
+      <c r="D30" s="152">
+        <v>0</v>
+      </c>
+      <c r="E30" s="151">
+        <v>0</v>
+      </c>
+      <c r="F30" s="152">
+        <v>0</v>
+      </c>
+      <c r="G30" s="151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="156">
+        <v>2116</v>
+      </c>
+      <c r="C31" s="157">
+        <v>0</v>
+      </c>
+      <c r="D31" s="152">
+        <v>0</v>
+      </c>
+      <c r="E31" s="151">
+        <v>0</v>
+      </c>
+      <c r="F31" s="152">
+        <v>0</v>
+      </c>
+      <c r="G31" s="151">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14114,7 +14838,7 @@
       <c r="E8" s="121">
         <v>22</v>
       </c>
-      <c r="F8" s="138">
+      <c r="F8" s="124">
         <v>170907119</v>
       </c>
       <c r="G8" s="121">
@@ -14143,7 +14867,7 @@
       <c r="E9" s="114">
         <v>29</v>
       </c>
-      <c r="F9" s="139">
+      <c r="F9" s="125">
         <v>-708502016</v>
       </c>
       <c r="G9" s="114">
@@ -14172,7 +14896,7 @@
       <c r="E10" s="115">
         <v>15</v>
       </c>
-      <c r="F10" s="140">
+      <c r="F10" s="126">
         <v>45090011</v>
       </c>
       <c r="G10" s="115">
@@ -14201,7 +14925,7 @@
       <c r="E11" s="115">
         <v>15</v>
       </c>
-      <c r="F11" s="140">
+      <c r="F11" s="126">
         <v>186383774</v>
       </c>
       <c r="G11" s="115">
@@ -14230,7 +14954,7 @@
       <c r="E12" s="115">
         <v>27</v>
       </c>
-      <c r="F12" s="140">
+      <c r="F12" s="126">
         <v>1559364</v>
       </c>
       <c r="G12" s="115">
@@ -14259,7 +14983,7 @@
       <c r="E13" s="115">
         <v>15</v>
       </c>
-      <c r="F13" s="140">
+      <c r="F13" s="126">
         <v>186609704</v>
       </c>
       <c r="G13" s="115">
@@ -14288,7 +15012,7 @@
       <c r="E14" s="115">
         <v>26</v>
       </c>
-      <c r="F14" s="140">
+      <c r="F14" s="126">
         <v>363842159</v>
       </c>
       <c r="G14" s="115">
@@ -14317,7 +15041,7 @@
       <c r="E15" s="115">
         <v>20</v>
       </c>
-      <c r="F15" s="140">
+      <c r="F15" s="126">
         <v>239527934</v>
       </c>
       <c r="G15" s="115">
@@ -14346,7 +15070,7 @@
       <c r="E16" s="115">
         <v>20</v>
       </c>
-      <c r="F16" s="140">
+      <c r="F16" s="126">
         <v>74325698</v>
       </c>
       <c r="G16" s="115">
@@ -14375,7 +15099,7 @@
       <c r="E17" s="115">
         <v>20</v>
       </c>
-      <c r="F17" s="140">
+      <c r="F17" s="126">
         <v>-213508592</v>
       </c>
       <c r="G17" s="115">
@@ -14404,7 +15128,7 @@
       <c r="E18" s="115">
         <v>25</v>
       </c>
-      <c r="F18" s="140">
+      <c r="F18" s="126">
         <v>-65987717</v>
       </c>
       <c r="G18" s="115">
@@ -14433,7 +15157,7 @@
       <c r="E19" s="115">
         <v>20</v>
       </c>
-      <c r="F19" s="141">
+      <c r="F19" s="127">
         <v>-288914220</v>
       </c>
       <c r="G19" s="115">
@@ -14462,7 +15186,7 @@
       <c r="E20" s="114">
         <v>14</v>
       </c>
-      <c r="F20" s="139">
+      <c r="F20" s="125">
         <v>-8169236</v>
       </c>
       <c r="G20" s="114">
@@ -14491,7 +15215,7 @@
       <c r="E21" s="115">
         <v>15</v>
       </c>
-      <c r="F21" s="140">
+      <c r="F21" s="126">
         <v>166625</v>
       </c>
       <c r="G21" s="115">
@@ -14520,7 +15244,7 @@
       <c r="E22" s="115">
         <v>15</v>
       </c>
-      <c r="F22" s="140">
+      <c r="F22" s="126">
         <v>-3743077</v>
       </c>
       <c r="G22" s="115">
@@ -14549,7 +15273,7 @@
       <c r="E23" s="115">
         <v>17</v>
       </c>
-      <c r="F23" s="140">
+      <c r="F23" s="126">
         <v>1803591</v>
       </c>
       <c r="G23" s="115">
@@ -14578,7 +15302,7 @@
       <c r="E24" s="115">
         <v>20</v>
       </c>
-      <c r="F24" s="140">
+      <c r="F24" s="126">
         <v>-18086022</v>
       </c>
       <c r="G24" s="115">
@@ -14607,7 +15331,7 @@
       <c r="E25" s="115">
         <v>21</v>
       </c>
-      <c r="F25" s="140">
+      <c r="F25" s="126">
         <v>2637271</v>
       </c>
       <c r="G25" s="115">
@@ -14636,7 +15360,7 @@
       <c r="E26" s="115">
         <v>21</v>
       </c>
-      <c r="F26" s="140">
+      <c r="F26" s="126">
         <v>-17048086</v>
       </c>
       <c r="G26" s="115">
@@ -14665,7 +15389,7 @@
       <c r="E27" s="115">
         <v>23</v>
       </c>
-      <c r="F27" s="140">
+      <c r="F27" s="126">
         <v>5526362</v>
       </c>
       <c r="G27" s="115">
@@ -14694,7 +15418,7 @@
       <c r="E28" s="115">
         <v>23</v>
       </c>
-      <c r="F28" s="140">
+      <c r="F28" s="126">
         <v>9294733</v>
       </c>
       <c r="G28" s="115">
@@ -14723,7 +15447,7 @@
       <c r="E29" s="115">
         <v>25</v>
       </c>
-      <c r="F29" s="140">
+      <c r="F29" s="126">
         <v>1009291</v>
       </c>
       <c r="G29" s="115">
@@ -14752,7 +15476,7 @@
       <c r="E30" s="115">
         <v>11</v>
       </c>
-      <c r="F30" s="140">
+      <c r="F30" s="126">
         <v>-6513673</v>
       </c>
       <c r="G30" s="115">
@@ -14781,7 +15505,7 @@
       <c r="E31" s="115">
         <v>26</v>
       </c>
-      <c r="F31" s="140">
+      <c r="F31" s="126">
         <v>-31736428</v>
       </c>
       <c r="G31" s="115">
@@ -14810,7 +15534,7 @@
       <c r="E32" s="115">
         <v>12</v>
       </c>
-      <c r="F32" s="140">
+      <c r="F32" s="126">
         <v>32874358</v>
       </c>
       <c r="G32" s="115">
@@ -14839,7 +15563,7 @@
       <c r="E33" s="115">
         <v>13</v>
       </c>
-      <c r="F33" s="140">
+      <c r="F33" s="126">
         <v>62698016</v>
       </c>
       <c r="G33" s="115">
@@ -14868,7 +15592,7 @@
       <c r="E34" s="115">
         <v>14</v>
       </c>
-      <c r="F34" s="140">
+      <c r="F34" s="126">
         <v>5166265</v>
       </c>
       <c r="G34" s="115">
@@ -14897,7 +15621,7 @@
       <c r="E35" s="115">
         <v>29</v>
       </c>
-      <c r="F35" s="140">
+      <c r="F35" s="126">
         <v>-10055165</v>
       </c>
       <c r="G35" s="115">
@@ -14926,7 +15650,7 @@
       <c r="E36" s="115">
         <v>15</v>
       </c>
-      <c r="F36" s="140">
+      <c r="F36" s="126">
         <v>12875476</v>
       </c>
       <c r="G36" s="115">
@@ -14955,7 +15679,7 @@
       <c r="E37" s="115">
         <v>30</v>
       </c>
-      <c r="F37" s="140">
+      <c r="F37" s="126">
         <v>32026629</v>
       </c>
       <c r="G37" s="115">
@@ -14984,7 +15708,7 @@
       <c r="E38" s="115">
         <v>15</v>
       </c>
-      <c r="F38" s="140">
+      <c r="F38" s="126">
         <v>10992586</v>
       </c>
       <c r="G38" s="115">
@@ -15013,7 +15737,7 @@
       <c r="E39" s="115">
         <v>30</v>
       </c>
-      <c r="F39" s="140">
+      <c r="F39" s="126">
         <v>33977506</v>
       </c>
       <c r="G39" s="115">
@@ -15042,7 +15766,7 @@
       <c r="E40" s="115">
         <v>21</v>
       </c>
-      <c r="F40" s="140">
+      <c r="F40" s="126">
         <v>-20388022</v>
       </c>
       <c r="G40" s="115">
@@ -15071,7 +15795,7 @@
       <c r="E41" s="115">
         <v>30</v>
       </c>
-      <c r="F41" s="140">
+      <c r="F41" s="126">
         <v>-5761499</v>
       </c>
       <c r="G41" s="115">
@@ -15100,7 +15824,7 @@
       <c r="E42" s="114">
         <v>17</v>
       </c>
-      <c r="F42" s="139">
+      <c r="F42" s="125">
         <v>-16018591</v>
       </c>
       <c r="G42" s="114">
@@ -15129,7 +15853,7 @@
       <c r="E43" s="115">
         <v>30</v>
       </c>
-      <c r="F43" s="140">
+      <c r="F43" s="126">
         <v>9093221</v>
       </c>
       <c r="G43" s="115">
@@ -15158,7 +15882,7 @@
       <c r="E44" s="115">
         <v>15</v>
       </c>
-      <c r="F44" s="140">
+      <c r="F44" s="126">
         <v>8570512</v>
       </c>
       <c r="G44" s="115">
@@ -15187,7 +15911,7 @@
       <c r="E45" s="115">
         <v>15</v>
       </c>
-      <c r="F45" s="140">
+      <c r="F45" s="126">
         <v>1896643</v>
       </c>
       <c r="G45" s="115">
@@ -15216,7 +15940,7 @@
       <c r="E46" s="115">
         <v>30</v>
       </c>
-      <c r="F46" s="140">
+      <c r="F46" s="126">
         <v>28549757</v>
       </c>
       <c r="G46" s="115">
@@ -15245,7 +15969,7 @@
       <c r="E47" s="115">
         <v>30</v>
       </c>
-      <c r="F47" s="140">
+      <c r="F47" s="126">
         <v>-19490</v>
       </c>
       <c r="G47" s="115">
@@ -15274,7 +15998,7 @@
       <c r="E48" s="115">
         <v>15</v>
       </c>
-      <c r="F48" s="140">
+      <c r="F48" s="126">
         <v>1006485</v>
       </c>
       <c r="G48" s="115">
@@ -15303,7 +16027,7 @@
       <c r="E49" s="115">
         <v>30</v>
       </c>
-      <c r="F49" s="140">
+      <c r="F49" s="126">
         <v>27643126</v>
       </c>
       <c r="G49" s="115">
@@ -15332,7 +16056,7 @@
       <c r="E50" s="115">
         <v>20</v>
       </c>
-      <c r="F50" s="140">
+      <c r="F50" s="126">
         <v>11032691</v>
       </c>
       <c r="G50" s="115">
@@ -15361,7 +16085,7 @@
       <c r="E51" s="115">
         <v>20</v>
       </c>
-      <c r="F51" s="140">
+      <c r="F51" s="126">
         <v>6042484</v>
       </c>
       <c r="G51" s="115">
@@ -15390,7 +16114,7 @@
       <c r="E52" s="115">
         <v>20</v>
       </c>
-      <c r="F52" s="140">
+      <c r="F52" s="126">
         <v>-15653324</v>
       </c>
       <c r="G52" s="115">
@@ -15419,7 +16143,7 @@
       <c r="E53" s="115">
         <v>25</v>
       </c>
-      <c r="F53" s="140">
+      <c r="F53" s="126">
         <v>-3574147</v>
       </c>
       <c r="G53" s="115">
@@ -15448,7 +16172,7 @@
       <c r="E54" s="115">
         <v>20</v>
       </c>
-      <c r="F54" s="141">
+      <c r="F54" s="127">
         <v>-46361062</v>
       </c>
       <c r="G54" s="115">
@@ -15477,7 +16201,7 @@
       <c r="E55" s="114">
         <v>14</v>
       </c>
-      <c r="F55" s="139">
+      <c r="F55" s="125">
         <v>-3201873</v>
       </c>
       <c r="G55" s="114">
@@ -15506,7 +16230,7 @@
       <c r="E56" s="115">
         <v>15</v>
       </c>
-      <c r="F56" s="140">
+      <c r="F56" s="126">
         <v>65309</v>
       </c>
       <c r="G56" s="115">
@@ -15535,7 +16259,7 @@
       <c r="E57" s="115">
         <v>15</v>
       </c>
-      <c r="F57" s="140">
+      <c r="F57" s="126">
         <v>-1467071</v>
       </c>
       <c r="G57" s="115">
@@ -15564,7 +16288,7 @@
       <c r="E58" s="115">
         <v>17</v>
       </c>
-      <c r="F58" s="140">
+      <c r="F58" s="126">
         <v>706904</v>
       </c>
       <c r="G58" s="115">
@@ -15593,7 +16317,7 @@
       <c r="E59" s="115">
         <v>20</v>
       </c>
-      <c r="F59" s="140">
+      <c r="F59" s="126">
         <v>-7088682</v>
       </c>
       <c r="G59" s="115">
@@ -15622,7 +16346,7 @@
       <c r="E60" s="115">
         <v>21</v>
       </c>
-      <c r="F60" s="140">
+      <c r="F60" s="126">
         <v>1033661</v>
       </c>
       <c r="G60" s="115">
@@ -15651,7 +16375,7 @@
       <c r="E61" s="115">
         <v>21</v>
       </c>
-      <c r="F61" s="140">
+      <c r="F61" s="126">
         <v>-6681874</v>
       </c>
       <c r="G61" s="115">
@@ -15680,7 +16404,7 @@
       <c r="E62" s="115">
         <v>23</v>
       </c>
-      <c r="F62" s="140">
+      <c r="F62" s="126">
         <v>2166018</v>
       </c>
       <c r="G62" s="115">
@@ -15709,7 +16433,7 @@
       <c r="E63" s="115">
         <v>23</v>
       </c>
-      <c r="F63" s="140">
+      <c r="F63" s="126">
         <v>3643005</v>
       </c>
       <c r="G63" s="115">
@@ -15738,7 +16462,7 @@
       <c r="E64" s="115">
         <v>25</v>
       </c>
-      <c r="F64" s="140">
+      <c r="F64" s="126">
         <v>393281</v>
       </c>
       <c r="G64" s="115">
@@ -15767,7 +16491,7 @@
       <c r="E65" s="115">
         <v>11</v>
       </c>
-      <c r="F65" s="140">
+      <c r="F65" s="126">
         <v>-1506076</v>
       </c>
       <c r="G65" s="115">
@@ -15796,7 +16520,7 @@
       <c r="E66" s="115">
         <v>26</v>
       </c>
-      <c r="F66" s="140">
+      <c r="F66" s="126">
         <v>-5311867</v>
       </c>
       <c r="G66" s="115">
@@ -15825,7 +16549,7 @@
       <c r="E67" s="115">
         <v>12</v>
       </c>
-      <c r="F67" s="140">
+      <c r="F67" s="126">
         <v>5538977</v>
       </c>
       <c r="G67" s="115">
@@ -15854,7 +16578,7 @@
       <c r="E68" s="115">
         <v>13</v>
       </c>
-      <c r="F68" s="140">
+      <c r="F68" s="126">
         <v>24673184</v>
       </c>
       <c r="G68" s="115">
@@ -15883,7 +16607,7 @@
       <c r="E69" s="115">
         <v>14</v>
       </c>
-      <c r="F69" s="140">
+      <c r="F69" s="126">
         <v>5188202</v>
       </c>
       <c r="G69" s="115">
@@ -15912,7 +16636,7 @@
       <c r="E70" s="115">
         <v>29</v>
       </c>
-      <c r="F70" s="140">
+      <c r="F70" s="126">
         <v>-6035109</v>
       </c>
       <c r="G70" s="115">
@@ -15941,7 +16665,7 @@
       <c r="E71" s="115">
         <v>15</v>
       </c>
-      <c r="F71" s="140">
+      <c r="F71" s="126">
         <v>7892672</v>
       </c>
       <c r="G71" s="115">
@@ -15970,7 +16694,7 @@
       <c r="E72" s="115">
         <v>30</v>
       </c>
-      <c r="F72" s="140">
+      <c r="F72" s="126">
         <v>16490896</v>
       </c>
       <c r="G72" s="115">
@@ -15999,7 +16723,7 @@
       <c r="E73" s="115">
         <v>15</v>
       </c>
-      <c r="F73" s="140">
+      <c r="F73" s="126">
         <v>4064244</v>
       </c>
       <c r="G73" s="115">
@@ -16028,7 +16752,7 @@
       <c r="E74" s="115">
         <v>30</v>
       </c>
-      <c r="F74" s="140">
+      <c r="F74" s="126">
         <v>16863317</v>
       </c>
       <c r="G74" s="115">
@@ -16057,7 +16781,7 @@
       <c r="E75" s="115">
         <v>21</v>
       </c>
-      <c r="F75" s="140">
+      <c r="F75" s="126">
         <v>-8693261</v>
       </c>
       <c r="G75" s="115">
@@ -16086,7 +16810,7 @@
       <c r="E76" s="115">
         <v>30</v>
       </c>
-      <c r="F76" s="140">
+      <c r="F76" s="126">
         <v>-3455996</v>
       </c>
       <c r="G76" s="115">
@@ -16115,7 +16839,7 @@
       <c r="E77" s="114">
         <v>17</v>
       </c>
-      <c r="F77" s="139">
+      <c r="F77" s="125">
         <v>-3878895</v>
       </c>
       <c r="G77" s="114">
@@ -16144,7 +16868,7 @@
       <c r="E78" s="115">
         <v>30</v>
       </c>
-      <c r="F78" s="140">
+      <c r="F78" s="126">
         <v>11996135</v>
       </c>
       <c r="G78" s="115">
@@ -16173,7 +16897,7 @@
       <c r="E79" s="115">
         <v>15</v>
       </c>
-      <c r="F79" s="140">
+      <c r="F79" s="126">
         <v>10060922</v>
       </c>
       <c r="G79" s="115">
@@ -16202,7 +16926,7 @@
       <c r="E80" s="115">
         <v>15</v>
       </c>
-      <c r="F80" s="140">
+      <c r="F80" s="126">
         <v>4239921</v>
       </c>
       <c r="G80" s="115">
@@ -16231,7 +16955,7 @@
       <c r="E81" s="115">
         <v>30</v>
       </c>
-      <c r="F81" s="140">
+      <c r="F81" s="126">
         <v>14219285</v>
       </c>
       <c r="G81" s="115">
@@ -16260,7 +16984,7 @@
       <c r="E82" s="115">
         <v>30</v>
       </c>
-      <c r="F82" s="140">
+      <c r="F82" s="126">
         <v>1601883</v>
       </c>
       <c r="G82" s="115">
@@ -16289,7 +17013,7 @@
       <c r="E83" s="115">
         <v>15</v>
       </c>
-      <c r="F83" s="140">
+      <c r="F83" s="126">
         <v>5391388</v>
       </c>
       <c r="G83" s="115">
@@ -16318,7 +17042,7 @@
       <c r="E84" s="115">
         <v>30</v>
       </c>
-      <c r="F84" s="140">
+      <c r="F84" s="126">
         <v>13774906</v>
       </c>
       <c r="G84" s="115">
@@ -16347,7 +17071,7 @@
       <c r="E85" s="115">
         <v>20</v>
       </c>
-      <c r="F85" s="140">
+      <c r="F85" s="126">
         <v>9419696</v>
       </c>
       <c r="G85" s="115">
@@ -16376,7 +17100,7 @@
       <c r="E86" s="115">
         <v>20</v>
       </c>
-      <c r="F86" s="140">
+      <c r="F86" s="126">
         <v>6659284</v>
       </c>
       <c r="G86" s="115">
@@ -16405,7 +17129,7 @@
       <c r="E87" s="115">
         <v>20</v>
       </c>
-      <c r="F87" s="140">
+      <c r="F87" s="126">
         <v>-11090879</v>
       </c>
       <c r="G87" s="115">
@@ -16434,7 +17158,7 @@
       <c r="E88" s="115">
         <v>25</v>
       </c>
-      <c r="F88" s="140">
+      <c r="F88" s="126">
         <v>10116212</v>
       </c>
       <c r="G88" s="115">
@@ -16463,7 +17187,7 @@
       <c r="E89" s="115">
         <v>20</v>
       </c>
-      <c r="F89" s="141">
+      <c r="F89" s="127">
         <v>-16640244</v>
       </c>
       <c r="G89" s="115">
@@ -16492,7 +17216,7 @@
       <c r="E90" s="114">
         <v>27</v>
       </c>
-      <c r="F90" s="139">
+      <c r="F90" s="125">
         <v>-175359657</v>
       </c>
       <c r="G90" s="114">
@@ -16521,7 +17245,7 @@
       <c r="E91" s="115">
         <v>13</v>
       </c>
-      <c r="F91" s="140">
+      <c r="F91" s="126">
         <v>-129982707</v>
       </c>
       <c r="G91" s="115">
@@ -16550,7 +17274,7 @@
       <c r="E92" s="115">
         <v>14</v>
       </c>
-      <c r="F92" s="140">
+      <c r="F92" s="126">
         <v>54451853</v>
       </c>
       <c r="G92" s="115">
@@ -16579,7 +17303,7 @@
       <c r="E93" s="115">
         <v>29</v>
       </c>
-      <c r="F93" s="140">
+      <c r="F93" s="126">
         <v>-279907155</v>
       </c>
       <c r="G93" s="115">
@@ -16608,7 +17332,7 @@
       <c r="E94" s="115">
         <v>15</v>
       </c>
-      <c r="F94" s="140">
+      <c r="F94" s="126">
         <v>144126876</v>
       </c>
       <c r="G94" s="115">
@@ -16637,7 +17361,7 @@
       <c r="E95" s="115">
         <v>30</v>
       </c>
-      <c r="F95" s="140">
+      <c r="F95" s="126">
         <v>494740512</v>
       </c>
       <c r="G95" s="115">
@@ -16666,7 +17390,7 @@
       <c r="E96" s="115">
         <v>15</v>
       </c>
-      <c r="F96" s="140">
+      <c r="F96" s="126">
         <v>42914963</v>
       </c>
       <c r="G96" s="115">
@@ -16695,7 +17419,7 @@
       <c r="E97" s="115">
         <v>30</v>
       </c>
-      <c r="F97" s="140">
+      <c r="F97" s="126">
         <v>337443657</v>
       </c>
       <c r="G97" s="115">
@@ -16724,7 +17448,7 @@
       <c r="E98" s="115">
         <v>21</v>
       </c>
-      <c r="F98" s="140">
+      <c r="F98" s="126">
         <v>-195732314</v>
       </c>
       <c r="G98" s="115">
@@ -16753,7 +17477,7 @@
       <c r="E99" s="115">
         <v>30</v>
       </c>
-      <c r="F99" s="140">
+      <c r="F99" s="126">
         <v>-81664512</v>
       </c>
       <c r="G99" s="115">
@@ -16782,7 +17506,7 @@
       <c r="E100" s="115">
         <v>17</v>
       </c>
-      <c r="F100" s="140">
+      <c r="F100" s="126">
         <v>-69561879</v>
       </c>
       <c r="G100" s="115">
@@ -16811,7 +17535,7 @@
       <c r="E101" s="115">
         <v>30</v>
       </c>
-      <c r="F101" s="140">
+      <c r="F101" s="126">
         <v>353871292</v>
       </c>
       <c r="G101" s="115">
@@ -16840,7 +17564,7 @@
       <c r="E102" s="115">
         <v>15</v>
       </c>
-      <c r="F102" s="140">
+      <c r="F102" s="126">
         <v>301419495</v>
       </c>
       <c r="G102" s="115">
@@ -16869,7 +17593,7 @@
       <c r="E103" s="115">
         <v>15</v>
       </c>
-      <c r="F103" s="140">
+      <c r="F103" s="126">
         <v>183599531</v>
       </c>
       <c r="G103" s="115">
@@ -16898,7 +17622,7 @@
       <c r="E104" s="115">
         <v>30</v>
       </c>
-      <c r="F104" s="140">
+      <c r="F104" s="126">
         <v>304932284</v>
       </c>
       <c r="G104" s="115">
@@ -16927,7 +17651,7 @@
       <c r="E105" s="115">
         <v>30</v>
       </c>
-      <c r="F105" s="140">
+      <c r="F105" s="126">
         <v>6149437</v>
       </c>
       <c r="G105" s="115">
@@ -16956,7 +17680,7 @@
       <c r="E106" s="115">
         <v>15</v>
       </c>
-      <c r="F106" s="140">
+      <c r="F106" s="126">
         <v>115045890</v>
       </c>
       <c r="G106" s="115">
@@ -17015,7 +17739,7 @@
       <c r="E107" s="115">
         <v>30</v>
       </c>
-      <c r="F107" s="140">
+      <c r="F107" s="126">
         <v>264201033</v>
       </c>
       <c r="G107" s="115">
@@ -17044,7 +17768,7 @@
       <c r="E108" s="115">
         <v>20</v>
       </c>
-      <c r="F108" s="140">
+      <c r="F108" s="126">
         <v>249737761</v>
       </c>
       <c r="G108" s="115">
@@ -17073,7 +17797,7 @@
       <c r="E109" s="115">
         <v>20</v>
       </c>
-      <c r="F109" s="140">
+      <c r="F109" s="126">
         <v>115981341</v>
       </c>
       <c r="G109" s="115">
@@ -17105,7 +17829,7 @@
       <c r="E110" s="115">
         <v>20</v>
       </c>
-      <c r="F110" s="140">
+      <c r="F110" s="126">
         <v>-247086097</v>
       </c>
       <c r="G110" s="115">
@@ -17134,7 +17858,7 @@
       <c r="E111" s="115">
         <v>25</v>
       </c>
-      <c r="F111" s="140">
+      <c r="F111" s="126">
         <v>36356826</v>
       </c>
       <c r="G111" s="115">
@@ -17163,7 +17887,7 @@
       <c r="E112" s="112">
         <v>20</v>
       </c>
-      <c r="F112" s="142">
+      <c r="F112" s="128">
         <v>-458582182</v>
       </c>
       <c r="G112" s="112">
@@ -17192,7 +17916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ERC cap before demographics
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo.xlsx
+++ b/Data_inputs/LAFPP_PlanInfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="268">
   <si>
     <t>Notes</t>
   </si>
@@ -1566,9 +1566,6 @@
     <t>EEC.rate</t>
   </si>
   <si>
-    <t>K12</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -2278,6 +2275,12 @@
   </si>
   <si>
     <t>Only model this type.</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>K13</t>
   </si>
 </sst>
 </file>
@@ -8925,13 +8928,13 @@
     </row>
     <row r="5" spans="1:8" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="143" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" s="98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="98" t="s">
         <v>263</v>
-      </c>
-      <c r="D5" s="98" t="s">
-        <v>264</v>
       </c>
       <c r="E5" s="158" t="s">
         <v>196</v>
@@ -8967,7 +8970,7 @@
     </row>
     <row r="7" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="144" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" s="95" t="s">
         <v>188</v>
@@ -9005,7 +9008,7 @@
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="89" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" s="96"/>
       <c r="E9" s="96"/>
@@ -9087,10 +9090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9117,7 +9120,7 @@
         <v>87</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9362,6 +9365,41 @@
         <v>0.09</v>
       </c>
       <c r="K12" s="88">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="88">
+        <v>20</v>
+      </c>
+      <c r="C13" s="88">
+        <v>50</v>
+      </c>
+      <c r="D13" s="88">
+        <v>2</v>
+      </c>
+      <c r="E13" s="88">
+        <v>0.03</v>
+      </c>
+      <c r="F13" s="88">
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="88">
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="88">
+        <v>50</v>
+      </c>
+      <c r="I13" s="88">
+        <v>20</v>
+      </c>
+      <c r="J13" s="88">
+        <v>0.09</v>
+      </c>
+      <c r="K13" s="88">
         <v>33</v>
       </c>
     </row>
@@ -14087,7 +14125,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -14095,47 +14133,47 @@
         <v>87</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" x14ac:dyDescent="0.25">
       <c r="B5" s="128" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="129" t="s">
         <v>249</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="D5" s="129" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="129" t="s">
+      <c r="E5" s="129" t="s">
         <v>251</v>
       </c>
-      <c r="E5" s="129" t="s">
+      <c r="F5" s="129" t="s">
         <v>252</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="G5" s="129" t="s">
         <v>253</v>
-      </c>
-      <c r="G5" s="129" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B6" s="130" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="131" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="131" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="E6" s="131" t="s">
         <v>256</v>
       </c>
-      <c r="E6" s="131" t="s">
+      <c r="F6" s="131" t="s">
         <v>257</v>
       </c>
-      <c r="F6" s="131" t="s">
+      <c r="G6" s="131" t="s">
         <v>258</v>
-      </c>
-      <c r="G6" s="131" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -14697,7 +14735,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -14736,7 +14774,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14753,7 +14791,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C8" s="18"/>
     </row>
@@ -15097,16 +15135,16 @@
         <v>87</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="114"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -15114,28 +15152,28 @@
     </row>
     <row r="6" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B6" s="101" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="102" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="D6" s="110" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="E6" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="F6" s="110" t="s">
         <v>212</v>
       </c>
-      <c r="F6" s="110" t="s">
+      <c r="G6" s="110" t="s">
         <v>213</v>
       </c>
-      <c r="G6" s="110" t="s">
-        <v>214</v>
-      </c>
       <c r="H6" s="112" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15143,28 +15181,28 @@
         <v>153</v>
       </c>
       <c r="B7" s="116" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="117" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="D7" s="118" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="E7" s="118" t="s">
         <v>229</v>
       </c>
-      <c r="E7" s="118" t="s">
+      <c r="F7" s="118" t="s">
         <v>230</v>
       </c>
-      <c r="F7" s="118" t="s">
+      <c r="G7" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="G7" s="118" t="s">
+      <c r="H7" s="119" t="s">
         <v>232</v>
       </c>
-      <c r="H7" s="119" t="s">
-        <v>233</v>
-      </c>
       <c r="I7" s="122" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15172,7 +15210,7 @@
         <v>154</v>
       </c>
       <c r="B8" s="103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" s="107">
         <v>42185</v>
@@ -15193,7 +15231,7 @@
         <v>14974146</v>
       </c>
       <c r="I8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15201,7 +15239,7 @@
         <v>155</v>
       </c>
       <c r="B9" s="103" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" s="107">
         <v>39629</v>
@@ -15222,7 +15260,7 @@
         <v>-44598831</v>
       </c>
       <c r="I9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15230,7 +15268,7 @@
         <v>155</v>
       </c>
       <c r="B10" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10" s="108">
         <v>39994</v>
@@ -15251,7 +15289,7 @@
         <v>5698407</v>
       </c>
       <c r="I10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15259,7 +15297,7 @@
         <v>155</v>
       </c>
       <c r="B11" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" s="108">
         <v>40359</v>
@@ -15280,7 +15318,7 @@
         <v>21534522</v>
       </c>
       <c r="I11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15288,7 +15326,7 @@
         <v>155</v>
       </c>
       <c r="B12" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C12" s="108">
         <v>40359</v>
@@ -15309,7 +15347,7 @@
         <v>98159</v>
       </c>
       <c r="I12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15317,7 +15355,7 @@
         <v>155</v>
       </c>
       <c r="B13" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13" s="108">
         <v>40724</v>
@@ -15338,7 +15376,7 @@
         <v>19908600</v>
       </c>
       <c r="I13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15346,7 +15384,7 @@
         <v>155</v>
       </c>
       <c r="B14" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" s="108">
         <v>40724</v>
@@ -15367,7 +15405,7 @@
         <v>22903160</v>
       </c>
       <c r="I14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15375,7 +15413,7 @@
         <v>155</v>
       </c>
       <c r="B15" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="108">
         <v>41090</v>
@@ -15396,7 +15434,7 @@
         <v>18122308</v>
       </c>
       <c r="I15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15404,7 +15442,7 @@
         <v>155</v>
       </c>
       <c r="B16" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16" s="108">
         <v>41455</v>
@@ -15425,7 +15463,7 @@
         <v>5391012</v>
       </c>
       <c r="I16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15433,7 +15471,7 @@
         <v>155</v>
       </c>
       <c r="B17" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C17" s="108">
         <v>41820</v>
@@ -15454,7 +15492,7 @@
         <v>-14891008</v>
       </c>
       <c r="I17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15462,7 +15500,7 @@
         <v>155</v>
       </c>
       <c r="B18" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" s="108">
         <v>41820</v>
@@ -15483,7 +15521,7 @@
         <v>-3919453</v>
       </c>
       <c r="I18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15491,7 +15529,7 @@
         <v>155</v>
       </c>
       <c r="B19" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C19" s="108">
         <v>42185</v>
@@ -15512,7 +15550,7 @@
         <v>-19427680</v>
       </c>
       <c r="I19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15520,7 +15558,7 @@
         <v>156</v>
       </c>
       <c r="B20" s="103" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C20" s="107">
         <v>32689</v>
@@ -15541,7 +15579,7 @@
         <v>-2144800</v>
       </c>
       <c r="I20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15549,7 +15587,7 @@
         <v>156</v>
       </c>
       <c r="B21" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C21" s="108">
         <v>33054</v>
@@ -15570,7 +15608,7 @@
         <v>35567</v>
       </c>
       <c r="I21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15578,7 +15616,7 @@
         <v>156</v>
       </c>
       <c r="B22" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" s="108">
         <v>33054</v>
@@ -15599,7 +15637,7 @@
         <v>-798975</v>
       </c>
       <c r="I22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15607,7 +15645,7 @@
         <v>156</v>
       </c>
       <c r="B23" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C23" s="108">
         <v>33785</v>
@@ -15628,7 +15666,7 @@
         <v>283932</v>
       </c>
       <c r="I23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15636,7 +15674,7 @@
         <v>156</v>
       </c>
       <c r="B24" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C24" s="108">
         <v>34880</v>
@@ -15657,7 +15695,7 @@
         <v>-2089634</v>
       </c>
       <c r="I24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15665,7 +15703,7 @@
         <v>156</v>
       </c>
       <c r="B25" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C25" s="108">
         <v>35246</v>
@@ -15686,7 +15724,7 @@
         <v>281359</v>
       </c>
       <c r="I25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15694,7 +15732,7 @@
         <v>156</v>
       </c>
       <c r="B26" s="104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="108">
         <v>35246</v>
@@ -15715,7 +15753,7 @@
         <v>-1818788</v>
       </c>
       <c r="I26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15723,7 +15761,7 @@
         <v>156</v>
       </c>
       <c r="B27" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" s="108">
         <v>35976</v>
@@ -15744,7 +15782,7 @@
         <v>514542</v>
       </c>
       <c r="I27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15752,7 +15790,7 @@
         <v>156</v>
       </c>
       <c r="B28" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="108">
         <v>35976</v>
@@ -15773,7 +15811,7 @@
         <v>865404</v>
       </c>
       <c r="I28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15781,7 +15819,7 @@
         <v>156</v>
       </c>
       <c r="B29" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C29" s="108">
         <v>36707</v>
@@ -15802,7 +15840,7 @@
         <v>83969</v>
       </c>
       <c r="I29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15810,7 +15848,7 @@
         <v>156</v>
       </c>
       <c r="B30" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C30" s="108">
         <v>37072</v>
@@ -15831,7 +15869,7 @@
         <v>-6513673</v>
       </c>
       <c r="I30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15839,7 +15877,7 @@
         <v>156</v>
       </c>
       <c r="B31" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C31" s="108">
         <v>37072</v>
@@ -15860,7 +15898,7 @@
         <v>-2513088</v>
       </c>
       <c r="I31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15868,7 +15906,7 @@
         <v>156</v>
       </c>
       <c r="B32" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32" s="108">
         <v>37437</v>
@@ -15889,7 +15927,7 @@
         <v>16709189</v>
       </c>
       <c r="I32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15897,7 +15935,7 @@
         <v>156</v>
       </c>
       <c r="B33" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C33" s="108">
         <v>37802</v>
@@ -15918,7 +15956,7 @@
         <v>21594795</v>
       </c>
       <c r="I33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15926,7 +15964,7 @@
         <v>156</v>
       </c>
       <c r="B34" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C34" s="108">
         <v>38168</v>
@@ -15947,7 +15985,7 @@
         <v>1356382</v>
       </c>
       <c r="I34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15955,7 +15993,7 @@
         <v>156</v>
       </c>
       <c r="B35" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C35" s="108">
         <v>38168</v>
@@ -15976,7 +16014,7 @@
         <v>-701290</v>
       </c>
       <c r="I35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15984,7 +16022,7 @@
         <v>156</v>
       </c>
       <c r="B36" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C36" s="108">
         <v>38533</v>
@@ -16005,7 +16043,7 @@
         <v>2748323</v>
       </c>
       <c r="I36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16013,7 +16051,7 @@
         <v>156</v>
       </c>
       <c r="B37" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C37" s="108">
         <v>38533</v>
@@ -16034,7 +16072,7 @@
         <v>2153591</v>
       </c>
       <c r="I37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16042,7 +16080,7 @@
         <v>156</v>
       </c>
       <c r="B38" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C38" s="108">
         <v>38898</v>
@@ -16063,7 +16101,7 @@
         <v>1986977</v>
       </c>
       <c r="I38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16071,7 +16109,7 @@
         <v>156</v>
       </c>
       <c r="B39" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C39" s="108">
         <v>38898</v>
@@ -16092,7 +16130,7 @@
         <v>2208183</v>
       </c>
       <c r="I39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16100,7 +16138,7 @@
         <v>156</v>
       </c>
       <c r="B40" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C40" s="108">
         <v>39263</v>
@@ -16121,7 +16159,7 @@
         <v>-1898265</v>
       </c>
       <c r="I40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16129,7 +16167,7 @@
         <v>156</v>
       </c>
       <c r="B41" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C41" s="108">
         <v>39263</v>
@@ -16150,7 +16188,7 @@
         <v>-362675</v>
       </c>
       <c r="I41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16158,7 +16196,7 @@
         <v>156</v>
       </c>
       <c r="B42" s="103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C42" s="107">
         <v>39629</v>
@@ -16179,7 +16217,7 @@
         <v>-1850766</v>
       </c>
       <c r="I42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16187,7 +16225,7 @@
         <v>156</v>
       </c>
       <c r="B43" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C43" s="108">
         <v>39629</v>
@@ -16208,7 +16246,7 @@
         <v>555518</v>
       </c>
       <c r="I43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16216,7 +16254,7 @@
         <v>156</v>
       </c>
       <c r="B44" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C44" s="108">
         <v>39994</v>
@@ -16237,7 +16275,7 @@
         <v>1083128</v>
       </c>
       <c r="I44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16245,7 +16283,7 @@
         <v>156</v>
       </c>
       <c r="B45" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C45" s="108">
         <v>40359</v>
@@ -16266,7 +16304,7 @@
         <v>219135</v>
       </c>
       <c r="I45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16274,7 +16312,7 @@
         <v>156</v>
       </c>
       <c r="B46" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C46" s="108">
         <v>40359</v>
@@ -16295,7 +16333,7 @@
         <v>1651439</v>
       </c>
       <c r="I46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16303,7 +16341,7 @@
         <v>156</v>
       </c>
       <c r="B47" s="104" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="108">
         <v>40724</v>
@@ -16324,7 +16362,7 @@
         <v>-1100</v>
       </c>
       <c r="I47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16332,7 +16370,7 @@
         <v>156</v>
       </c>
       <c r="B48" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" s="108">
         <v>40724</v>
@@ -16353,7 +16391,7 @@
         <v>107378</v>
       </c>
       <c r="I48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16361,7 +16399,7 @@
         <v>156</v>
       </c>
       <c r="B49" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C49" s="108">
         <v>40724</v>
@@ -16382,7 +16420,7 @@
         <v>1559561</v>
       </c>
       <c r="I49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16390,7 +16428,7 @@
         <v>156</v>
       </c>
       <c r="B50" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C50" s="108">
         <v>41090</v>
@@ -16411,7 +16449,7 @@
         <v>834716</v>
       </c>
       <c r="I50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16419,7 +16457,7 @@
         <v>156</v>
       </c>
       <c r="B51" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C51" s="108">
         <v>41455</v>
@@ -16440,7 +16478,7 @@
         <v>438275</v>
       </c>
       <c r="I51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16448,7 +16486,7 @@
         <v>156</v>
       </c>
       <c r="B52" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C52" s="108">
         <v>41820</v>
@@ -16469,7 +16507,7 @@
         <v>-1091730</v>
       </c>
       <c r="I52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16477,7 +16515,7 @@
         <v>156</v>
       </c>
       <c r="B53" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C53" s="108">
         <v>41820</v>
@@ -16498,7 +16536,7 @@
         <v>-212293</v>
       </c>
       <c r="I53" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16506,7 +16544,7 @@
         <v>156</v>
       </c>
       <c r="B54" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C54" s="108">
         <v>42185</v>
@@ -16527,7 +16565,7 @@
         <v>-3117492</v>
       </c>
       <c r="I54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16535,7 +16573,7 @@
         <v>157</v>
       </c>
       <c r="B55" s="103" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C55" s="107">
         <v>32689</v>
@@ -16556,7 +16594,7 @@
         <v>-840639</v>
       </c>
       <c r="I55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16564,7 +16602,7 @@
         <v>157</v>
       </c>
       <c r="B56" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C56" s="108">
         <v>33054</v>
@@ -16585,7 +16623,7 @@
         <v>13940</v>
       </c>
       <c r="I56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16593,7 +16631,7 @@
         <v>157</v>
       </c>
       <c r="B57" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C57" s="108">
         <v>33054</v>
@@ -16614,7 +16652,7 @@
         <v>-313152</v>
       </c>
       <c r="I57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16622,7 +16660,7 @@
         <v>157</v>
       </c>
       <c r="B58" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C58" s="108">
         <v>33785</v>
@@ -16643,7 +16681,7 @@
         <v>111285</v>
       </c>
       <c r="I58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16651,7 +16689,7 @@
         <v>157</v>
       </c>
       <c r="B59" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C59" s="108">
         <v>34880</v>
@@ -16672,7 +16710,7 @@
         <v>-819016</v>
       </c>
       <c r="I59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16680,7 +16718,7 @@
         <v>157</v>
       </c>
       <c r="B60" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C60" s="108">
         <v>35246</v>
@@ -16701,7 +16739,7 @@
         <v>110277</v>
       </c>
       <c r="I60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16709,7 +16747,7 @@
         <v>157</v>
       </c>
       <c r="B61" s="104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C61" s="108">
         <v>35246</v>
@@ -16730,7 +16768,7 @@
         <v>-712861</v>
       </c>
       <c r="I61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16738,7 +16776,7 @@
         <v>157</v>
       </c>
       <c r="B62" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C62" s="108">
         <v>35976</v>
@@ -16759,7 +16797,7 @@
         <v>201671</v>
       </c>
       <c r="I62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16767,7 +16805,7 @@
         <v>157</v>
       </c>
       <c r="B63" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C63" s="108">
         <v>35976</v>
@@ -16788,7 +16826,7 @@
         <v>339189</v>
       </c>
       <c r="I63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16796,7 +16834,7 @@
         <v>157</v>
       </c>
       <c r="B64" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C64" s="108">
         <v>36707</v>
@@ -16817,7 +16855,7 @@
         <v>32719</v>
       </c>
       <c r="I64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16825,7 +16863,7 @@
         <v>157</v>
       </c>
       <c r="B65" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C65" s="108">
         <v>37072</v>
@@ -16846,7 +16884,7 @@
         <v>-1506076</v>
       </c>
       <c r="I65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16854,7 +16892,7 @@
         <v>157</v>
       </c>
       <c r="B66" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C66" s="108">
         <v>37072</v>
@@ -16875,7 +16913,7 @@
         <v>-420627</v>
       </c>
       <c r="I66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16883,7 +16921,7 @@
         <v>157</v>
       </c>
       <c r="B67" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C67" s="108">
         <v>37437</v>
@@ -16904,7 +16942,7 @@
         <v>2815319</v>
       </c>
       <c r="I67" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16912,7 +16950,7 @@
         <v>157</v>
       </c>
       <c r="B68" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C68" s="108">
         <v>37802</v>
@@ -16933,7 +16971,7 @@
         <v>8498073</v>
       </c>
       <c r="I68" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16941,7 +16979,7 @@
         <v>157</v>
       </c>
       <c r="B69" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C69" s="108">
         <v>38168</v>
@@ -16962,7 +17000,7 @@
         <v>1362141</v>
       </c>
       <c r="I69" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16970,7 +17008,7 @@
         <v>157</v>
       </c>
       <c r="B70" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C70" s="108">
         <v>38168</v>
@@ -16991,7 +17029,7 @@
         <v>-420914</v>
       </c>
       <c r="I70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16999,7 +17037,7 @@
         <v>157</v>
       </c>
       <c r="B71" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C71" s="108">
         <v>38533</v>
@@ -17020,7 +17058,7 @@
         <v>1684723</v>
       </c>
       <c r="I71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17028,7 +17066,7 @@
         <v>157</v>
       </c>
       <c r="B72" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C72" s="108">
         <v>38533</v>
@@ -17049,7 +17087,7 @@
         <v>1108910</v>
       </c>
       <c r="I72" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17057,7 +17095,7 @@
         <v>157</v>
       </c>
       <c r="B73" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C73" s="108">
         <v>38898</v>
@@ -17078,7 +17116,7 @@
         <v>734637</v>
       </c>
       <c r="I73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17086,7 +17124,7 @@
         <v>157</v>
       </c>
       <c r="B74" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C74" s="108">
         <v>38898</v>
@@ -17107,7 +17145,7 @@
         <v>1095940</v>
       </c>
       <c r="I74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17115,7 +17153,7 @@
         <v>157</v>
       </c>
       <c r="B75" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C75" s="108">
         <v>39263</v>
@@ -17136,7 +17174,7 @@
         <v>-809403</v>
       </c>
       <c r="I75" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17144,7 +17182,7 @@
         <v>157</v>
       </c>
       <c r="B76" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C76" s="108">
         <v>39263</v>
@@ -17165,7 +17203,7 @@
         <v>-217548</v>
       </c>
       <c r="I76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17173,7 +17211,7 @@
         <v>157</v>
       </c>
       <c r="B77" s="103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C77" s="107">
         <v>39629</v>
@@ -17194,7 +17232,7 @@
         <v>-448162</v>
       </c>
       <c r="I77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17202,7 +17240,7 @@
         <v>157</v>
       </c>
       <c r="B78" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C78" s="108">
         <v>39629</v>
@@ -17223,7 +17261,7 @@
         <v>732862</v>
       </c>
       <c r="I78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17231,7 +17269,7 @@
         <v>157</v>
       </c>
       <c r="B79" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C79" s="108">
         <v>39994</v>
@@ -17252,7 +17290,7 @@
         <v>1271484</v>
       </c>
       <c r="I79" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17260,7 +17298,7 @@
         <v>157</v>
       </c>
       <c r="B80" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C80" s="108">
         <v>40359</v>
@@ -17281,7 +17319,7 @@
         <v>489875</v>
       </c>
       <c r="I80" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17289,7 +17327,7 @@
         <v>157</v>
       </c>
       <c r="B81" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C81" s="108">
         <v>40359</v>
@@ -17310,7 +17348,7 @@
         <v>822504</v>
       </c>
       <c r="I81" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17318,7 +17356,7 @@
         <v>157</v>
       </c>
       <c r="B82" s="104" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C82" s="108">
         <v>40724</v>
@@ -17339,7 +17377,7 @@
         <v>90375</v>
       </c>
       <c r="I82" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17347,7 +17385,7 @@
         <v>157</v>
       </c>
       <c r="B83" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C83" s="108">
         <v>40724</v>
@@ -17368,7 +17406,7 @@
         <v>575184</v>
       </c>
       <c r="I83" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17376,7 +17414,7 @@
         <v>157</v>
       </c>
       <c r="B84" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C84" s="108">
         <v>40724</v>
@@ -17397,7 +17435,7 @@
         <v>777148</v>
       </c>
       <c r="I84" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17405,7 +17443,7 @@
         <v>157</v>
       </c>
       <c r="B85" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C85" s="108">
         <v>41090</v>
@@ -17426,7 +17464,7 @@
         <v>712679</v>
       </c>
       <c r="I85" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17434,7 +17472,7 @@
         <v>157</v>
       </c>
       <c r="B86" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C86" s="108">
         <v>41455</v>
@@ -17455,7 +17493,7 @@
         <v>483013</v>
       </c>
       <c r="I86" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17463,7 +17501,7 @@
         <v>157</v>
       </c>
       <c r="B87" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C87" s="108">
         <v>41820</v>
@@ -17484,7 +17522,7 @@
         <v>-773526</v>
       </c>
       <c r="I87" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17492,7 +17530,7 @@
         <v>157</v>
       </c>
       <c r="B88" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C88" s="108">
         <v>41820</v>
@@ -17513,7 +17551,7 @@
         <v>600870</v>
       </c>
       <c r="I88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17521,7 +17559,7 @@
         <v>157</v>
       </c>
       <c r="B89" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C89" s="108">
         <v>42185</v>
@@ -17542,7 +17580,7 @@
         <v>-1118953</v>
       </c>
       <c r="I89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17550,7 +17588,7 @@
         <v>158</v>
       </c>
       <c r="B90" s="103" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C90" s="107">
         <v>37437</v>
@@ -17571,7 +17609,7 @@
         <v>-13267437</v>
       </c>
       <c r="I90" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17579,7 +17617,7 @@
         <v>158</v>
       </c>
       <c r="B91" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C91" s="108">
         <v>37802</v>
@@ -17600,7 +17638,7 @@
         <v>-44769357</v>
       </c>
       <c r="I91" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17608,7 +17646,7 @@
         <v>158</v>
       </c>
       <c r="B92" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C92" s="108">
         <v>38168</v>
@@ -17629,7 +17667,7 @@
         <v>14296114</v>
       </c>
       <c r="I92" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17637,7 +17675,7 @@
         <v>158</v>
       </c>
       <c r="B93" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C93" s="108">
         <v>38168</v>
@@ -17658,7 +17696,7 @@
         <v>-19521929</v>
       </c>
       <c r="I93" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17666,7 +17704,7 @@
         <v>158</v>
       </c>
       <c r="B94" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C94" s="108">
         <v>38533</v>
@@ -17687,7 +17725,7 @@
         <v>30764476</v>
       </c>
       <c r="I94" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17695,7 +17733,7 @@
         <v>158</v>
       </c>
       <c r="B95" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C95" s="108">
         <v>38533</v>
@@ -17716,7 +17754,7 @@
         <v>33268214</v>
       </c>
       <c r="I95" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17724,7 +17762,7 @@
         <v>158</v>
       </c>
       <c r="B96" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C96" s="108">
         <v>38898</v>
@@ -17745,7 +17783,7 @@
         <v>7757140</v>
       </c>
       <c r="I96" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17753,7 +17791,7 @@
         <v>158</v>
       </c>
       <c r="B97" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C97" s="108">
         <v>38898</v>
@@ -17774,7 +17812,7 @@
         <v>21930315</v>
       </c>
       <c r="I97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17782,7 +17820,7 @@
         <v>158</v>
       </c>
       <c r="B98" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C98" s="108">
         <v>39263</v>
@@ -17803,7 +17841,7 @@
         <v>-18224028</v>
       </c>
       <c r="I98" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="99" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17811,7 +17849,7 @@
         <v>158</v>
       </c>
       <c r="B99" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" s="108">
         <v>39263</v>
@@ -17832,7 +17870,7 @@
         <v>-5140623</v>
       </c>
       <c r="I99" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17840,7 +17878,7 @@
         <v>158</v>
       </c>
       <c r="B100" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C100" s="108">
         <v>39629</v>
@@ -17861,7 +17899,7 @@
         <v>-8037083</v>
       </c>
       <c r="I100" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="101" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17869,7 +17907,7 @@
         <v>158</v>
       </c>
       <c r="B101" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C101" s="108">
         <v>39629</v>
@@ -17890,7 +17928,7 @@
         <v>21618528</v>
       </c>
       <c r="I101" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17898,7 +17936,7 @@
         <v>158</v>
       </c>
       <c r="B102" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C102" s="108">
         <v>39994</v>
@@ -17919,7 +17957,7 @@
         <v>38092937</v>
       </c>
       <c r="I102" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="103" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17927,7 +17965,7 @@
         <v>158</v>
       </c>
       <c r="B103" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C103" s="108">
         <v>40359</v>
@@ -17948,7 +17986,7 @@
         <v>21212834</v>
       </c>
       <c r="I103" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17956,7 +17994,7 @@
         <v>158</v>
       </c>
       <c r="B104" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C104" s="108">
         <v>40359</v>
@@ -17977,7 +18015,7 @@
         <v>17638581</v>
       </c>
       <c r="I104" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -17985,7 +18023,7 @@
         <v>158</v>
       </c>
       <c r="B105" s="104" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C105" s="108">
         <v>40724</v>
@@ -18006,7 +18044,7 @@
         <v>346937</v>
       </c>
       <c r="I105" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18014,7 +18052,7 @@
         <v>158</v>
       </c>
       <c r="B106" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C106" s="108">
         <v>40724</v>
@@ -18035,19 +18073,19 @@
         <v>12273760</v>
       </c>
       <c r="I106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L106" s="106" t="s">
+        <v>233</v>
+      </c>
+      <c r="M106" t="s">
         <v>234</v>
       </c>
-      <c r="M106" t="s">
+      <c r="N106" t="s">
         <v>235</v>
       </c>
-      <c r="N106" t="s">
+      <c r="O106" t="s">
         <v>236</v>
-      </c>
-      <c r="O106" t="s">
-        <v>237</v>
       </c>
       <c r="P106" s="29">
         <v>42185</v>
@@ -18073,7 +18111,7 @@
         <v>158</v>
       </c>
       <c r="B107" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C107" s="108">
         <v>40724</v>
@@ -18094,7 +18132,7 @@
         <v>14905607</v>
       </c>
       <c r="I107" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="108" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18102,7 +18140,7 @@
         <v>159</v>
       </c>
       <c r="B108" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C108" s="108">
         <v>41090</v>
@@ -18123,7 +18161,7 @@
         <v>18894767</v>
       </c>
       <c r="I108" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18131,7 +18169,7 @@
         <v>159</v>
       </c>
       <c r="B109" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C109" s="108">
         <v>41455</v>
@@ -18152,7 +18190,7 @@
         <v>8412390</v>
       </c>
       <c r="I109" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O109" s="30"/>
       <c r="Q109" s="30"/>
@@ -18163,7 +18201,7 @@
         <v>159</v>
       </c>
       <c r="B110" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C110" s="108">
         <v>41820</v>
@@ -18184,7 +18222,7 @@
         <v>-17232847</v>
       </c>
       <c r="I110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18192,7 +18230,7 @@
         <v>159</v>
       </c>
       <c r="B111" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C111" s="108">
         <v>41820</v>
@@ -18213,7 +18251,7 @@
         <v>2159476</v>
       </c>
       <c r="I111" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18221,7 +18259,7 @@
         <v>159</v>
       </c>
       <c r="B112" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C112" s="109">
         <v>42185</v>
@@ -18242,7 +18280,7 @@
         <v>-30836792</v>
       </c>
       <c r="I112" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
@@ -18283,7 +18321,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
@@ -18293,25 +18331,25 @@
         <v>87</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>